<commit_message>
update visualization of results - activity status & production
</commit_message>
<xml_diff>
--- a/data/new_file_lithiumsites.xlsx
+++ b/data/new_file_lithiumsites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schenker\PycharmProjects\Geothermal_brines\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96A4E2B-0DAE-49F7-9EF1-4B893C5173E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14154EBF-A94E-4FD1-8C6D-311F6D9E66A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
+    <workbookView xWindow="9518" yWindow="0" windowWidth="9765" windowHeight="10162" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6768,7 +6768,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
update visualization of results - Production & Li-conc
</commit_message>
<xml_diff>
--- a/data/new_file_lithiumsites.xlsx
+++ b/data/new_file_lithiumsites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schenker\PycharmProjects\Geothermal_brines\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14154EBF-A94E-4FD1-8C6D-311F6D9E66A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE61D5A-7A59-4025-BE55-8A6D018B1CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9518" yWindow="0" windowWidth="9765" windowHeight="10162" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4163" uniqueCount="1787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4164" uniqueCount="1787">
   <si>
     <t>Site name</t>
   </si>
@@ -5367,9 +5367,6 @@
     <t>activity_status</t>
   </si>
   <si>
-    <t>Limited production</t>
-  </si>
-  <si>
     <t>Feasibility complete</t>
   </si>
   <si>
@@ -5404,18 +5401,22 @@
   </si>
   <si>
     <t>Advanced exploration</t>
+  </si>
+  <si>
+    <t>sum_impurities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -5555,7 +5556,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5669,6 +5670,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -6767,8 +6774,8 @@
   <dimension ref="A1:AA96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92:XFD92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7050,82 +7057,82 @@
         <v>1773</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1774</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>1775</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>1776</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1785</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>1776</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>1776</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>1777</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="O4" s="1" t="s">
+        <v>1780</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>1778</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>1780</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>1779</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>1786</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>1777</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>1776</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>1778</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>1781</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>1779</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>1778</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>1779</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>1779</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="W4" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>1782</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>1781</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>1778</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>1776</v>
-      </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="Z4" s="1" t="s">
         <v>1783</v>
       </c>
-      <c r="Y4" s="1" t="s">
-        <v>1776</v>
-      </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>1784</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>1785</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.45">
@@ -9939,7 +9946,7 @@
         <v>2030000</v>
       </c>
       <c r="D49" s="10">
-        <v>70000000</v>
+        <v>202000000</v>
       </c>
       <c r="E49" s="11">
         <v>12605000</v>
@@ -12025,16 +12032,114 @@
       <c r="Z91" s="17"/>
       <c r="AA91" s="17"/>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="P92" s="17"/>
-      <c r="Q92" s="17"/>
-      <c r="R92" s="17"/>
-      <c r="S92" s="17"/>
-      <c r="T92" s="17"/>
-      <c r="U92" s="17"/>
-      <c r="V92" s="17"/>
-      <c r="W92" s="17"/>
-      <c r="Z92" s="17"/>
+    <row r="92" spans="1:27" s="42" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A92" s="43" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B92" s="42">
+        <f>SUM(B37:B41,B43,B44,B45)</f>
+        <v>2.610849557522124</v>
+      </c>
+      <c r="C92" s="42">
+        <f t="shared" ref="C92:AA92" si="21">SUM(C37:C41,C43,C44,C45)</f>
+        <v>0.49976106194690262</v>
+      </c>
+      <c r="D92" s="42">
+        <f>SUM(D37:D41,D43,D44,D45)</f>
+        <v>2.6019999999999999</v>
+      </c>
+      <c r="E92" s="42">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F92" s="42">
+        <f t="shared" si="21"/>
+        <v>3.694</v>
+      </c>
+      <c r="G92" s="42">
+        <f t="shared" si="21"/>
+        <v>2.9009121061359866</v>
+      </c>
+      <c r="H92" s="42">
+        <f t="shared" si="21"/>
+        <v>9.2113747383112354</v>
+      </c>
+      <c r="I92" s="42">
+        <f t="shared" si="21"/>
+        <v>1.6392622950819671</v>
+      </c>
+      <c r="J92" s="42">
+        <f t="shared" si="21"/>
+        <v>3.1279508196721308</v>
+      </c>
+      <c r="K92" s="42">
+        <f t="shared" si="21"/>
+        <v>1.2854918032786884</v>
+      </c>
+      <c r="L92" s="42">
+        <f t="shared" si="21"/>
+        <v>0.18733333333333332</v>
+      </c>
+      <c r="M92" s="42">
+        <f t="shared" si="21"/>
+        <v>1.0654228855721393</v>
+      </c>
+      <c r="N92" s="42">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="O92" s="42">
+        <f t="shared" si="21"/>
+        <v>9.2113747383112354</v>
+      </c>
+      <c r="P92" s="42">
+        <f t="shared" si="21"/>
+        <v>0.82327868852459019</v>
+      </c>
+      <c r="Q92" s="42">
+        <f t="shared" si="21"/>
+        <v>1.2222950819672129</v>
+      </c>
+      <c r="R92" s="42">
+        <f t="shared" si="21"/>
+        <v>0.82278688524590171</v>
+      </c>
+      <c r="S92" s="42">
+        <f t="shared" si="21"/>
+        <v>1.0522950819672132</v>
+      </c>
+      <c r="T92" s="42">
+        <f t="shared" si="21"/>
+        <v>0.42540983606557375</v>
+      </c>
+      <c r="U92" s="42">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V92" s="42">
+        <f>SUM(V37:V41,V43,V44,V45)</f>
+        <v>3.5024999999999999</v>
+      </c>
+      <c r="W92" s="42">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="X92" s="42">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="Y92" s="42">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="Z92" s="42">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AA92" s="42">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="1:27" x14ac:dyDescent="0.45">
       <c r="P93" s="17"/>

</xml_diff>

<commit_message>
Waterfall graphs & Marimekko graphs
</commit_message>
<xml_diff>
--- a/data/new_file_lithiumsites.xlsx
+++ b/data/new_file_lithiumsites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schenker\PycharmProjects\Geothermal_brines\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE61D5A-7A59-4025-BE55-8A6D018B1CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2049AB92-E923-4D88-A363-BCDBA47C64BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
   </bookViews>
@@ -5416,7 +5416,7 @@
     <numFmt numFmtId="165" formatCode="0.000000000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -5668,14 +5668,14 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -6771,11 +6771,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5319587E-5250-4C3E-BD3D-6C0619F44C22}">
-  <dimension ref="A1:AA96"/>
+  <dimension ref="A1:AA101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92:XFD92"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z72" sqref="Z72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10971,10 +10971,10 @@
         <v>156</v>
       </c>
       <c r="Y72" s="17" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="Z72" s="17" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="AA72" s="35" t="s">
         <v>156</v>
@@ -12032,111 +12032,111 @@
       <c r="Z91" s="17"/>
       <c r="AA91" s="17"/>
     </row>
-    <row r="92" spans="1:27" s="42" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="43" t="s">
+    <row r="92" spans="1:27" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A92" s="42" t="s">
         <v>1786</v>
       </c>
-      <c r="B92" s="42">
+      <c r="B92" s="41">
         <f>SUM(B37:B41,B43,B44,B45)</f>
         <v>2.610849557522124</v>
       </c>
-      <c r="C92" s="42">
+      <c r="C92" s="41">
         <f t="shared" ref="C92:AA92" si="21">SUM(C37:C41,C43,C44,C45)</f>
         <v>0.49976106194690262</v>
       </c>
-      <c r="D92" s="42">
+      <c r="D92" s="41">
         <f>SUM(D37:D41,D43,D44,D45)</f>
         <v>2.6019999999999999</v>
       </c>
-      <c r="E92" s="42">
+      <c r="E92" s="41">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="F92" s="42">
+      <c r="F92" s="41">
         <f t="shared" si="21"/>
         <v>3.694</v>
       </c>
-      <c r="G92" s="42">
+      <c r="G92" s="41">
         <f t="shared" si="21"/>
         <v>2.9009121061359866</v>
       </c>
-      <c r="H92" s="42">
+      <c r="H92" s="41">
         <f t="shared" si="21"/>
         <v>9.2113747383112354</v>
       </c>
-      <c r="I92" s="42">
+      <c r="I92" s="41">
         <f t="shared" si="21"/>
         <v>1.6392622950819671</v>
       </c>
-      <c r="J92" s="42">
+      <c r="J92" s="41">
         <f t="shared" si="21"/>
         <v>3.1279508196721308</v>
       </c>
-      <c r="K92" s="42">
+      <c r="K92" s="41">
         <f t="shared" si="21"/>
         <v>1.2854918032786884</v>
       </c>
-      <c r="L92" s="42">
+      <c r="L92" s="41">
         <f t="shared" si="21"/>
         <v>0.18733333333333332</v>
       </c>
-      <c r="M92" s="42">
+      <c r="M92" s="41">
         <f t="shared" si="21"/>
         <v>1.0654228855721393</v>
       </c>
-      <c r="N92" s="42">
+      <c r="N92" s="41">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="O92" s="42">
+      <c r="O92" s="41">
         <f t="shared" si="21"/>
         <v>9.2113747383112354</v>
       </c>
-      <c r="P92" s="42">
+      <c r="P92" s="41">
         <f t="shared" si="21"/>
         <v>0.82327868852459019</v>
       </c>
-      <c r="Q92" s="42">
+      <c r="Q92" s="41">
         <f t="shared" si="21"/>
         <v>1.2222950819672129</v>
       </c>
-      <c r="R92" s="42">
+      <c r="R92" s="41">
         <f t="shared" si="21"/>
         <v>0.82278688524590171</v>
       </c>
-      <c r="S92" s="42">
+      <c r="S92" s="41">
         <f t="shared" si="21"/>
         <v>1.0522950819672132</v>
       </c>
-      <c r="T92" s="42">
+      <c r="T92" s="41">
         <f t="shared" si="21"/>
         <v>0.42540983606557375</v>
       </c>
-      <c r="U92" s="42">
+      <c r="U92" s="41">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="V92" s="42">
+      <c r="V92" s="41">
         <f>SUM(V37:V41,V43,V44,V45)</f>
         <v>3.5024999999999999</v>
       </c>
-      <c r="W92" s="42">
+      <c r="W92" s="41">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="X92" s="42">
+      <c r="X92" s="41">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="Y92" s="42">
+      <c r="Y92" s="41">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="Z92" s="42">
+      <c r="Z92" s="41">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AA92" s="42">
+      <c r="AA92" s="41">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -12184,6 +12184,12 @@
       <c r="V96" s="17"/>
       <c r="W96" s="17"/>
       <c r="Z96" s="17"/>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E101" s="1">
+        <f>E66</f>
+        <v>128340</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -13187,18 +13193,18 @@
       <c r="B3" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="43" t="s">
         <v>242</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Output tables & class ResourceCalculator
</commit_message>
<xml_diff>
--- a/data/new_file_lithiumsites.xlsx
+++ b/data/new_file_lithiumsites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schenker\PycharmProjects\Geothermal_brines\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11191D8-30F2-4929-BFE1-253B067405DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7542A3D-8749-41BB-B249-9127F1F79654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet4!$A$2:$A$278</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet4!$B$2:$B$278</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet4!$A$2:$A$282</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet4!$B$2:$B$282</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4146" uniqueCount="1786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="1791">
   <si>
     <t>Site name</t>
   </si>
@@ -5388,9 +5388,6 @@
     <t>Reserves Development</t>
   </si>
   <si>
-    <t>Feasibility started</t>
-  </si>
-  <si>
     <t>Commissioning</t>
   </si>
   <si>
@@ -5401,6 +5398,24 @@
   </si>
   <si>
     <t>sum_impurities</t>
+  </si>
+  <si>
+    <t>Feasibility Started</t>
+  </si>
+  <si>
+    <t>Ang_1</t>
+  </si>
+  <si>
+    <t>Ang_2</t>
+  </si>
+  <si>
+    <t>Ang_3</t>
+  </si>
+  <si>
+    <t>Ang_4</t>
+  </si>
+  <si>
+    <t>Sal del Los Angeles</t>
   </si>
 </sst>
 </file>
@@ -5553,7 +5568,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5674,6 +5689,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5738,677 +5755,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
-      </cx:strDim>
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{7D417D07-6795-4C63-8F0E-631EF745056A}">
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="0"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>292892</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Chart 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86B354E5-BF55-4416-89A1-A2A752B83CAE}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="7203280" y="0"/>
-              <a:ext cx="5860257" cy="3200400"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF265331-BEA9-4E55-863B-C6CFAA95AB8B}" name="Table1" displayName="Table1" ref="A1:Q278" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:Q278" xr:uid="{AF265331-BEA9-4E55-863B-C6CFAA95AB8B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF265331-BEA9-4E55-863B-C6CFAA95AB8B}" name="Table1" displayName="Table1" ref="A1:Q282" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:Q282" xr:uid="{AF265331-BEA9-4E55-863B-C6CFAA95AB8B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q278">
     <sortCondition ref="A1:A278"/>
   </sortState>
@@ -6768,11 +6117,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5319587E-5250-4C3E-BD3D-6C0619F44C22}">
-  <dimension ref="A1:Z101"/>
+  <dimension ref="A1:AL101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M65" sqref="M65"/>
+      <selection pane="bottomLeft" activeCell="Z50" sqref="Z50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6790,13 +6139,16 @@
     <col min="13" max="13" width="13.1328125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.265625" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="9.1328125" style="1"/>
+    <col min="16" max="18" width="9.1328125" style="1"/>
+    <col min="19" max="19" width="27.33203125" style="1" customWidth="1"/>
     <col min="20" max="20" width="13.1328125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.1328125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.1328125" style="1"/>
+    <col min="25" max="25" width="9.1328125" style="1"/>
+    <col min="26" max="26" width="15.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.45">
@@ -7072,7 +6424,7 @@
         <v>1777</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>1775</v>
@@ -7108,16 +6460,16 @@
         <v>1774</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>1781</v>
+        <v>1785</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>1774</v>
       </c>
       <c r="Y4" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="Z4" s="1" t="s">
         <v>1782</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>1783</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.45">
@@ -7737,6 +7089,9 @@
       </c>
       <c r="Y13" s="1">
         <v>1.349</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>1.22</v>
       </c>
     </row>
     <row r="14" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
@@ -7855,7 +7210,10 @@
       <c r="Y15" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="Z15" s="17"/>
+      <c r="Z15" s="17">
+        <f>((Sheet2!Y2/1000)/(Sheet1!$Z$13*1000))*100</f>
+        <v>1.9262295081967213E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
@@ -7929,9 +7287,12 @@
       <c r="V16" s="1">
         <v>10.06</v>
       </c>
-      <c r="Z16" s="17"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="Z16" s="17">
+        <f>((Sheet2!Y3/1000)/(Sheet1!$Z$13*1000))*100</f>
+        <v>3.1368852459016399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>195</v>
       </c>
@@ -8003,9 +7364,12 @@
       <c r="V17" s="1">
         <v>6.2</v>
       </c>
-      <c r="Z17" s="17"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="Z17" s="17">
+        <f>((Sheet2!Y4/1000)/(Sheet1!$Z$13*1000))*100</f>
+        <v>1.7651639344262295</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>196</v>
       </c>
@@ -8083,9 +7447,21 @@
       <c r="V18" s="1">
         <v>0.8</v>
       </c>
-      <c r="Z18" s="17"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="Z18" s="17">
+        <f>((Sheet2!Y5/1000)/(Sheet1!$Z$13*1000))*100</f>
+        <v>0.64557377049180331</v>
+      </c>
+      <c r="AD18" s="44"/>
+      <c r="AE18" s="45"/>
+      <c r="AF18" s="45"/>
+      <c r="AG18" s="45"/>
+      <c r="AH18" s="45"/>
+      <c r="AI18" s="45"/>
+      <c r="AJ18" s="45"/>
+      <c r="AK18" s="45"/>
+      <c r="AL18" s="45"/>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
         <v>197</v>
       </c>
@@ -8160,9 +7536,12 @@
       <c r="V19" s="1">
         <v>0.71</v>
       </c>
-      <c r="Z19" s="17"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="Z19" s="17">
+        <f>((Sheet2!Y6/1000)/(Sheet1!$Z$13*1000))*100</f>
+        <v>0.11499999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
         <v>198</v>
       </c>
@@ -8243,9 +7622,12 @@
       <c r="V20" s="1">
         <v>0.02</v>
       </c>
-      <c r="Z20" s="17"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="Z20" s="17">
+        <f>((Sheet2!Y7/1000)/(Sheet1!$Z$13*1000))*100</f>
+        <v>7.6475409836065572E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
         <v>199</v>
       </c>
@@ -8283,7 +7665,7 @@
         <f>((Sheet2!E8/1000)/(Sheet1!$K$13*1000))*100</f>
         <v>0.86967213114754094</v>
       </c>
-      <c r="L21" s="17"/>
+      <c r="L21" s="35"/>
       <c r="M21" s="17">
         <f t="shared" si="0"/>
         <v>0.84436152570480927</v>
@@ -8320,9 +7702,12 @@
       <c r="V21" s="1">
         <v>0</v>
       </c>
-      <c r="Z21" s="17"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="Z21" s="17">
+        <f>((Sheet2!Y8/1000)/(Sheet1!$Z$13*1000))*100</f>
+        <v>0.78581967213114756</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>200</v>
       </c>
@@ -8400,9 +7785,12 @@
       <c r="V22" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Z22" s="17"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="Z22" s="17">
+        <f>((Sheet2!Y9/1000)/(Sheet1!$Z$13*1000))*100</f>
+        <v>6.6229508196721326E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>201</v>
       </c>
@@ -8435,7 +7823,7 @@
       </c>
       <c r="Z23" s="17"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>202</v>
       </c>
@@ -8468,7 +7856,7 @@
       </c>
       <c r="Z24" s="17"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>203</v>
       </c>
@@ -8501,7 +7889,7 @@
       </c>
       <c r="Z25" s="17"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>204</v>
       </c>
@@ -8534,7 +7922,7 @@
       </c>
       <c r="Z26" s="17"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>205</v>
       </c>
@@ -8567,7 +7955,7 @@
       </c>
       <c r="Z27" s="17"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>206</v>
       </c>
@@ -8600,7 +7988,7 @@
       </c>
       <c r="Z28" s="17"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>1762</v>
       </c>
@@ -8633,7 +8021,7 @@
       </c>
       <c r="Z29" s="17"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>207</v>
       </c>
@@ -8689,7 +8077,7 @@
       </c>
       <c r="R30" s="17">
         <f>Z30</f>
-        <v>0</v>
+        <v>93.389590163934429</v>
       </c>
       <c r="S30" s="17">
         <f>M30</f>
@@ -8707,9 +8095,12 @@
         <f>100 - SUM(V15:V29)</f>
         <v>82.185000000000002</v>
       </c>
-      <c r="Z30" s="17"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="Z30" s="17">
+        <f>100-SUM(Z15:Z22)</f>
+        <v>93.389590163934429</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
@@ -8789,8 +8180,11 @@
       <c r="Y31" s="1">
         <v>1.349</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="Z31" s="1">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
         <v>48</v>
       </c>
@@ -8810,6 +8204,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="Z32" s="19"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
@@ -8898,7 +8293,10 @@
       <c r="Y33" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="Z33" s="17"/>
+      <c r="Z33" s="17">
+        <f>Z15</f>
+        <v>1.9262295081967213E-2</v>
+      </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
@@ -8964,7 +8362,10 @@
         <f t="shared" si="5"/>
         <v>16.974999999999998</v>
       </c>
-      <c r="Z34" s="17"/>
+      <c r="Z34" s="17">
+        <f t="shared" ref="Z34:Z40" si="7">Z16</f>
+        <v>3.1368852459016399</v>
+      </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
@@ -8999,12 +8400,12 @@
         <v>2.0954918032786889</v>
       </c>
       <c r="K35" s="17">
-        <f t="shared" ref="K35" si="7">K17</f>
+        <f t="shared" ref="K35" si="8">K17</f>
         <v>7.5737704918032795</v>
       </c>
       <c r="L35" s="17"/>
       <c r="M35" s="19">
-        <f t="shared" ref="M35:M39" si="8">M17</f>
+        <f t="shared" ref="M35:M39" si="9">M17</f>
         <v>9.1776119402985081</v>
       </c>
       <c r="N35" s="17"/>
@@ -9030,7 +8431,10 @@
         <f t="shared" si="5"/>
         <v>8.7833333333333332</v>
       </c>
-      <c r="Z35" s="17"/>
+      <c r="Z35" s="17">
+        <f t="shared" si="7"/>
+        <v>1.7651639344262295</v>
+      </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
@@ -9065,12 +8469,12 @@
         <v>0.61827868852459023</v>
       </c>
       <c r="K36" s="17">
-        <f t="shared" ref="K36" si="9">K18</f>
+        <f t="shared" ref="K36" si="10">K18</f>
         <v>0.3040983606557377</v>
       </c>
       <c r="L36" s="17"/>
       <c r="M36" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.68101160862354893</v>
       </c>
       <c r="N36" s="17"/>
@@ -9096,7 +8500,10 @@
         <f t="shared" si="5"/>
         <v>1.3083333333333331</v>
       </c>
-      <c r="Z36" s="17"/>
+      <c r="Z36" s="17">
+        <f t="shared" si="7"/>
+        <v>0.64557377049180331</v>
+      </c>
     </row>
     <row r="37" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="23" t="s">
@@ -9131,15 +8538,15 @@
         <v>4.2377049180327871E-2</v>
       </c>
       <c r="K37" s="24">
-        <f t="shared" ref="K37" si="10">K19</f>
+        <f t="shared" ref="K37" si="11">K19</f>
         <v>6.5573770491803282E-2</v>
       </c>
       <c r="L37" s="24">
-        <f t="shared" ref="L37:L40" si="11">L19</f>
+        <f t="shared" ref="L37:L40" si="12">L19</f>
         <v>3.241666666666667E-2</v>
       </c>
       <c r="M37" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0696517412935316E-2</v>
       </c>
       <c r="N37" s="24"/>
@@ -9168,7 +8575,10 @@
         <f t="shared" si="5"/>
         <v>0.27750000000000002</v>
       </c>
-      <c r="Z37" s="24"/>
+      <c r="Z37" s="17">
+        <f t="shared" si="7"/>
+        <v>0.11499999999999999</v>
+      </c>
     </row>
     <row r="38" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="23" t="s">
@@ -9203,15 +8613,15 @@
         <v>0.33540983606557373</v>
       </c>
       <c r="K38" s="24">
-        <f t="shared" ref="K38" si="12">K20</f>
+        <f t="shared" ref="K38" si="13">K20</f>
         <v>0.21311475409836067</v>
       </c>
       <c r="L38" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.13633333333333331</v>
       </c>
       <c r="M38" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.15174129353233831</v>
       </c>
       <c r="N38" s="24"/>
@@ -9240,7 +8650,10 @@
         <f t="shared" si="5"/>
         <v>1.3916666666666666</v>
       </c>
-      <c r="Z38" s="24"/>
+      <c r="Z38" s="17">
+        <f t="shared" si="7"/>
+        <v>7.6475409836065572E-2</v>
+      </c>
     </row>
     <row r="39" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
@@ -9275,12 +8688,12 @@
         <v>2.4791803278688525</v>
       </c>
       <c r="K39" s="24">
-        <f t="shared" ref="K39" si="13">K21</f>
+        <f t="shared" ref="K39" si="14">K21</f>
         <v>0.86967213114754094</v>
       </c>
       <c r="L39" s="24"/>
       <c r="M39" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.84436152570480927</v>
       </c>
       <c r="N39" s="24"/>
@@ -9309,7 +8722,10 @@
         <f t="shared" si="5"/>
         <v>1.7750000000000001</v>
       </c>
-      <c r="Z39" s="24"/>
+      <c r="Z39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.78581967213114756</v>
+      </c>
     </row>
     <row r="40" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="23" t="s">
@@ -9344,11 +8760,11 @@
         <v>0.27098360655737708</v>
       </c>
       <c r="K40" s="24">
-        <f t="shared" ref="K40" si="14">K22</f>
+        <f t="shared" ref="K40" si="15">K22</f>
         <v>0.1371311475409836</v>
       </c>
       <c r="L40" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.8583333333333334E-2</v>
       </c>
       <c r="M40" s="24">
@@ -9381,7 +8797,10 @@
         <f t="shared" si="5"/>
         <v>5.8333333333333327E-2</v>
       </c>
-      <c r="Z40" s="24"/>
+      <c r="Z40" s="17">
+        <f t="shared" si="7"/>
+        <v>6.6229508196721326E-2</v>
+      </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
@@ -9451,7 +8870,7 @@
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
       <c r="M42" s="19">
-        <f t="shared" ref="M42:M48" si="15">M24</f>
+        <f t="shared" ref="M42:M48" si="16">M24</f>
         <v>0</v>
       </c>
       <c r="N42" s="17"/>
@@ -9499,7 +8918,7 @@
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
       <c r="M43" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N43" s="17"/>
@@ -9547,7 +8966,7 @@
       <c r="K44" s="17"/>
       <c r="L44" s="17"/>
       <c r="M44" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N44" s="17"/>
@@ -9595,7 +9014,7 @@
       <c r="K45" s="17"/>
       <c r="L45" s="17"/>
       <c r="M45" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N45" s="17"/>
@@ -9643,7 +9062,7 @@
       <c r="K46" s="17"/>
       <c r="L46" s="17"/>
       <c r="M46" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N46" s="17"/>
@@ -9691,7 +9110,7 @@
       <c r="K47" s="24"/>
       <c r="L47" s="24"/>
       <c r="M47" s="24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N47" s="24"/>
@@ -9701,15 +9120,15 @@
         <v>0</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" ref="Q47:S47" si="16">Q29</f>
+        <f t="shared" ref="Q47:S47" si="17">Q29</f>
         <v>0</v>
       </c>
       <c r="R47" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="S47" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T47" s="24"/>
@@ -9717,7 +9136,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z47" s="24"/>
+      <c r="Z47" s="17"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
@@ -9758,25 +9177,25 @@
       </c>
       <c r="L48" s="17"/>
       <c r="M48" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>74.067578772802662</v>
       </c>
       <c r="N48" s="17"/>
       <c r="O48" s="17"/>
       <c r="P48" s="1">
-        <f t="shared" ref="P48:S48" si="17">P30</f>
+        <f t="shared" ref="P48:S48" si="18">P30</f>
         <v>89.308688524590167</v>
       </c>
       <c r="Q48" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>78.597295081967218</v>
       </c>
       <c r="R48" s="1">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>93.389590163934429</v>
       </c>
       <c r="S48" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>74.067578772802662</v>
       </c>
       <c r="T48" s="17"/>
@@ -9784,7 +9203,10 @@
         <f t="shared" si="5"/>
         <v>69.360833333333332</v>
       </c>
-      <c r="Z48" s="17"/>
+      <c r="Z48" s="17">
+        <f>100-SUM(Z33:Z40)</f>
+        <v>93.389590163934429</v>
+      </c>
     </row>
     <row r="49" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
@@ -9838,6 +9260,9 @@
       <c r="X49" s="10">
         <v>10000000</v>
       </c>
+      <c r="Z49" s="10">
+        <v>20000000</v>
+      </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
@@ -10127,6 +9552,9 @@
       <c r="Y55" s="1">
         <v>0.77</v>
       </c>
+      <c r="Z55" s="1">
+        <v>0.77</v>
+      </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
@@ -10676,16 +10104,16 @@
         <v>167</v>
       </c>
       <c r="I71" s="17" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="J71" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="K71" s="35" t="s">
-        <v>152</v>
+      <c r="K71" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="L71" s="17" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="M71" s="17" t="s">
         <v>170</v>
@@ -10696,29 +10124,29 @@
       <c r="O71" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="P71" s="35" t="s">
-        <v>152</v>
+      <c r="P71" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="Q71" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="R71" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="S71" s="35" t="s">
-        <v>152</v>
+        <v>170</v>
+      </c>
+      <c r="R71" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="S71" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="T71" s="17" t="s">
         <v>168</v>
       </c>
       <c r="U71" s="17" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="V71" s="17" t="s">
         <v>169</v>
       </c>
       <c r="W71" s="17" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="X71" s="17" t="s">
         <v>152</v>
@@ -10726,8 +10154,8 @@
       <c r="Y71" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="Z71" s="35" t="s">
-        <v>152</v>
+      <c r="Z71" s="17" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -10755,17 +10183,17 @@
       <c r="H72" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="I72" s="17" t="s">
-        <v>156</v>
+      <c r="I72" s="35" t="s">
+        <v>151</v>
       </c>
       <c r="J72" s="17" t="s">
         <v>156</v>
       </c>
       <c r="K72" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="L72" s="17" t="s">
-        <v>156</v>
+        <v>151</v>
+      </c>
+      <c r="L72" s="35" t="s">
+        <v>151</v>
       </c>
       <c r="M72" s="35" t="s">
         <v>151</v>
@@ -10777,28 +10205,28 @@
         <v>169</v>
       </c>
       <c r="P72" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q72" s="17" t="s">
-        <v>156</v>
+        <v>151</v>
+      </c>
+      <c r="Q72" s="35" t="s">
+        <v>151</v>
       </c>
       <c r="R72" s="35" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="S72" s="35" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="T72" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="U72" s="17" t="s">
-        <v>156</v>
+      <c r="U72" s="35" t="s">
+        <v>151</v>
       </c>
       <c r="V72" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="W72" s="17" t="s">
-        <v>156</v>
+      <c r="W72" s="35" t="s">
+        <v>151</v>
       </c>
       <c r="X72" s="17" t="s">
         <v>154</v>
@@ -10807,7 +10235,7 @@
         <v>154</v>
       </c>
       <c r="Z72" s="35" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -10836,16 +10264,16 @@
         <v>170</v>
       </c>
       <c r="I73" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J73" s="17" t="s">
         <v>154</v>
       </c>
       <c r="K73" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L73" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M73" s="17" t="s">
         <v>152</v>
@@ -10857,28 +10285,28 @@
         <v>170</v>
       </c>
       <c r="P73" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q73" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="R73" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="S73" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="T73" s="17" t="s">
         <v>170</v>
       </c>
       <c r="U73" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="V73" s="17" t="s">
         <v>159</v>
       </c>
       <c r="W73" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="X73" s="17" t="s">
         <v>1765</v>
@@ -10887,7 +10315,7 @@
         <v>1765</v>
       </c>
       <c r="Z73" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -10916,16 +10344,16 @@
         <v>171</v>
       </c>
       <c r="I74" s="17" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="J74" s="17" t="s">
         <v>176</v>
       </c>
       <c r="K74" s="35" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="L74" s="17" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="M74" s="17" t="s">
         <v>156</v>
@@ -10937,28 +10365,28 @@
         <v>171</v>
       </c>
       <c r="P74" s="35" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="Q74" s="17" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="R74" s="35" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="S74" s="35" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="T74" s="17" t="s">
         <v>171</v>
       </c>
       <c r="U74" s="17" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="V74" s="17" t="s">
         <v>158</v>
       </c>
       <c r="W74" s="17" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="X74" s="17" t="s">
         <v>155</v>
@@ -10967,7 +10395,7 @@
         <v>155</v>
       </c>
       <c r="Z74" s="35" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -10996,16 +10424,16 @@
         <v>153</v>
       </c>
       <c r="I75" s="17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J75" s="17" t="s">
         <v>157</v>
       </c>
       <c r="K75" s="35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="L75" s="17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M75" s="17" t="s">
         <v>154</v>
@@ -11017,28 +10445,28 @@
         <v>172</v>
       </c>
       <c r="P75" s="35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q75" s="17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="R75" s="35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="S75" s="35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="T75" s="17" t="s">
         <v>172</v>
       </c>
       <c r="U75" s="17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="V75" s="17" t="s">
         <v>160</v>
       </c>
       <c r="W75" s="17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="X75" s="17" t="s">
         <v>176</v>
@@ -11047,7 +10475,7 @@
         <v>176</v>
       </c>
       <c r="Z75" s="35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -11076,16 +10504,16 @@
         <v>169</v>
       </c>
       <c r="I76" s="17" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="J76" s="17" t="s">
         <v>158</v>
       </c>
       <c r="K76" s="35" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="L76" s="17" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="M76" s="17" t="s">
         <v>176</v>
@@ -11097,28 +10525,28 @@
         <v>173</v>
       </c>
       <c r="P76" s="35" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="Q76" s="17" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="R76" s="35" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="S76" s="35" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="T76" s="17" t="s">
         <v>173</v>
       </c>
       <c r="U76" s="17" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="V76" s="17" t="s">
         <v>169</v>
       </c>
       <c r="W76" s="17" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="X76" s="17" t="s">
         <v>157</v>
@@ -11127,7 +10555,7 @@
         <v>157</v>
       </c>
       <c r="Z76" s="35" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -11156,16 +10584,16 @@
         <v>157</v>
       </c>
       <c r="I77" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J77" s="17" t="s">
         <v>159</v>
       </c>
       <c r="K77" s="35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L77" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M77" s="17" t="s">
         <v>157</v>
@@ -11177,28 +10605,28 @@
         <v>174</v>
       </c>
       <c r="P77" s="35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Q77" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="R77" s="35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="S77" s="35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="T77" s="17" t="s">
         <v>174</v>
       </c>
       <c r="U77" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="V77" s="17" t="s">
         <v>174</v>
       </c>
       <c r="W77" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="X77" s="17" t="s">
         <v>158</v>
@@ -11207,7 +10635,7 @@
         <v>158</v>
       </c>
       <c r="Z77" s="35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -11236,16 +10664,16 @@
         <v>158</v>
       </c>
       <c r="I78" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J78" s="17" t="s">
         <v>160</v>
       </c>
       <c r="K78" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L78" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="M78" s="17" t="s">
         <v>158</v>
@@ -11257,28 +10685,28 @@
         <v>157</v>
       </c>
       <c r="P78" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q78" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="R78" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="S78" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="T78" s="17" t="s">
         <v>157</v>
       </c>
       <c r="U78" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="V78" s="17" t="s">
         <v>174</v>
       </c>
       <c r="W78" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X78" s="17" t="s">
         <v>159</v>
@@ -11287,7 +10715,7 @@
         <v>159</v>
       </c>
       <c r="Z78" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -11316,16 +10744,16 @@
         <v>159</v>
       </c>
       <c r="I79" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J79" s="17" t="s">
         <v>161</v>
       </c>
       <c r="K79" s="35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L79" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M79" s="17" t="s">
         <v>159</v>
@@ -11337,28 +10765,28 @@
         <v>158</v>
       </c>
       <c r="P79" s="35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="Q79" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="R79" s="35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S79" s="35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T79" s="17" t="s">
         <v>158</v>
       </c>
       <c r="U79" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="V79" s="17" t="s">
         <v>154</v>
       </c>
       <c r="W79" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="X79" s="17" t="s">
         <v>160</v>
@@ -11367,7 +10795,7 @@
         <v>160</v>
       </c>
       <c r="Z79" s="35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -11396,16 +10824,16 @@
         <v>160</v>
       </c>
       <c r="I80" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J80" s="17" t="s">
         <v>162</v>
       </c>
       <c r="K80" s="35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L80" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M80" s="17" t="s">
         <v>160</v>
@@ -11417,28 +10845,28 @@
         <v>159</v>
       </c>
       <c r="P80" s="35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q80" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="R80" s="35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="S80" s="35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="T80" s="17" t="s">
         <v>159</v>
       </c>
       <c r="U80" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="V80" s="17" t="s">
         <v>161</v>
       </c>
       <c r="W80" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="X80" s="17" t="s">
         <v>161</v>
@@ -11447,7 +10875,7 @@
         <v>161</v>
       </c>
       <c r="Z80" s="35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -11476,16 +10904,16 @@
         <v>161</v>
       </c>
       <c r="I81" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J81" s="17" t="s">
         <v>163</v>
       </c>
       <c r="K81" s="35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L81" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M81" s="17" t="s">
         <v>161</v>
@@ -11497,28 +10925,28 @@
         <v>160</v>
       </c>
       <c r="P81" s="35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q81" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="R81" s="35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S81" s="35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="T81" s="17" t="s">
         <v>160</v>
       </c>
       <c r="U81" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="V81" s="17" t="s">
         <v>162</v>
       </c>
       <c r="W81" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="X81" s="17" t="s">
         <v>162</v>
@@ -11527,7 +10955,7 @@
         <v>162</v>
       </c>
       <c r="Z81" s="35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -11556,16 +10984,16 @@
         <v>162</v>
       </c>
       <c r="I82" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J82" s="17" t="s">
         <v>164</v>
       </c>
       <c r="K82" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L82" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="M82" s="17" t="s">
         <v>162</v>
@@ -11577,28 +11005,28 @@
         <v>161</v>
       </c>
       <c r="P82" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q82" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="R82" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="S82" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="T82" s="17" t="s">
         <v>161</v>
       </c>
       <c r="U82" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="V82" s="17" t="s">
         <v>163</v>
       </c>
       <c r="W82" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="X82" s="17" t="s">
         <v>163</v>
@@ -11607,7 +11035,7 @@
         <v>163</v>
       </c>
       <c r="Z82" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -11635,17 +11063,17 @@
       <c r="H83" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="I83" s="1" t="s">
-        <v>165</v>
+      <c r="I83" s="17" t="s">
+        <v>163</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="K83" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>165</v>
+      <c r="K83" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="L83" s="17" t="s">
+        <v>163</v>
       </c>
       <c r="M83" s="17" t="s">
         <v>163</v>
@@ -11653,29 +11081,29 @@
       <c r="O83" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="P83" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q83" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="R83" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="S83" s="14" t="s">
-        <v>165</v>
+      <c r="P83" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q83" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="R83" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="S83" s="35" t="s">
+        <v>163</v>
       </c>
       <c r="T83" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="U83" s="1" t="s">
-        <v>165</v>
+      <c r="U83" s="17" t="s">
+        <v>163</v>
       </c>
       <c r="V83" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="W83" s="1" t="s">
-        <v>165</v>
+      <c r="W83" s="17" t="s">
+        <v>163</v>
       </c>
       <c r="X83" s="17" t="s">
         <v>164</v>
@@ -11683,8 +11111,8 @@
       <c r="Y83" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="Z83" s="14" t="s">
-        <v>165</v>
+      <c r="Z83" s="35" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -11712,29 +11140,54 @@
       <c r="H84" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="K84" s="19"/>
+      <c r="I84" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="K84" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="L84" s="17" t="s">
+        <v>164</v>
+      </c>
       <c r="M84" s="17" t="s">
         <v>164</v>
       </c>
       <c r="O84" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="P84" s="19"/>
-      <c r="R84" s="19"/>
-      <c r="S84" s="19"/>
+      <c r="P84" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q84" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="R84" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="S84" s="35" t="s">
+        <v>164</v>
+      </c>
       <c r="T84" s="17" t="s">
         <v>163</v>
       </c>
+      <c r="U84" s="17" t="s">
+        <v>164</v>
+      </c>
       <c r="V84" s="1" t="s">
         <v>165</v>
       </c>
+      <c r="W84" s="17" t="s">
+        <v>164</v>
+      </c>
       <c r="X84" s="1" t="s">
         <v>165</v>
       </c>
       <c r="Y84" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="Z84" s="19"/>
+      <c r="Z84" s="35" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="85" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A85" s="20" t="s">
@@ -11758,14 +11211,44 @@
       <c r="H85" s="1" t="s">
         <v>165</v>
       </c>
+      <c r="I85" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K85" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="M85" s="1" t="s">
         <v>165</v>
       </c>
       <c r="O85" s="17" t="s">
         <v>164</v>
       </c>
+      <c r="P85" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q85" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="R85" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="S85" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="T85" s="17" t="s">
         <v>164</v>
+      </c>
+      <c r="U85" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="W85" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z85" s="14" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.45">
@@ -11835,14 +11318,14 @@
     </row>
     <row r="92" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A92" s="42" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="B92" s="41">
         <f>SUM(B37:B41,B43,B44,B45)</f>
         <v>2.610849557522124</v>
       </c>
       <c r="C92" s="41">
-        <f t="shared" ref="C92:Z92" si="18">SUM(C37:C41,C43,C44,C45)</f>
+        <f t="shared" ref="C92:Z92" si="19">SUM(C37:C41,C43,C44,C45)</f>
         <v>0.49976106194690262</v>
       </c>
       <c r="D92" s="41">
@@ -11850,67 +11333,67 @@
         <v>2.6019999999999999</v>
       </c>
       <c r="E92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3.694</v>
       </c>
       <c r="G92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2.9009121061359866</v>
       </c>
       <c r="H92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9.2113747383112354</v>
       </c>
       <c r="I92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.6392622950819671</v>
       </c>
       <c r="J92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3.1279508196721308</v>
       </c>
       <c r="K92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.2854918032786884</v>
       </c>
       <c r="L92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.18733333333333332</v>
       </c>
       <c r="M92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.0654228855721393</v>
       </c>
       <c r="N92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9.2113747383112354</v>
       </c>
       <c r="P92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.82327868852459019</v>
       </c>
       <c r="Q92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.2222950819672129</v>
       </c>
       <c r="R92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.0522950819672132</v>
       </c>
       <c r="S92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.42540983606557375</v>
       </c>
       <c r="T92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="U92" s="41">
@@ -11918,24 +11401,24 @@
         <v>3.5024999999999999</v>
       </c>
       <c r="V92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y92" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Z92" s="41">
-        <f t="shared" si="18"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1.0435245901639345</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.45">
@@ -11993,11 +11476,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80513011-51AC-48FD-950E-E3C602EF619D}">
-  <dimension ref="A1:X57"/>
+  <dimension ref="A1:Y57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N2" sqref="N2"/>
+      <selection pane="topRight" activeCell="Y2" sqref="Y2:Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12006,7 +11489,7 @@
     <col min="9" max="10" width="13.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -12079,8 +11562,11 @@
       <c r="X1" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y1" s="1" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -12127,8 +11613,11 @@
       <c r="Q2">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y2" s="45">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -12166,8 +11655,11 @@
       <c r="Q3">
         <v>203.7</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y3" s="45">
+        <v>38270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -12205,8 +11697,11 @@
       <c r="Q4">
         <v>105.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y4" s="45">
+        <v>21535</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -12250,8 +11745,11 @@
       <c r="Q5">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y5" s="45">
+        <v>7876</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -12292,8 +11790,11 @@
       <c r="Q6">
         <v>3.33</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y6" s="45">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -12340,8 +11841,11 @@
       <c r="Q7">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y7" s="45">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -12379,8 +11883,11 @@
       <c r="Q8">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y8" s="45">
+        <v>9587</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -12424,38 +11931,41 @@
       <c r="Q9">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y9" s="45">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -12974,15 +12484,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82018139-1009-4013-9ADC-EC34767F8B53}">
-  <dimension ref="A3:L592"/>
+  <dimension ref="A3:AA592"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A1:L1048576"/>
+      <selection activeCell="P6" sqref="P6:AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>240</v>
       </c>
@@ -12999,7 +12509,7 @@
       <c r="K3" s="43"/>
       <c r="L3" s="43"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>242</v>
       </c>
@@ -13037,12 +12547,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -13080,7 +12590,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>254</v>
       </c>
@@ -13117,8 +12627,18 @@
       <c r="L7">
         <v>302</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="R7" s="43"/>
+      <c r="S7" s="43"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="43"/>
+      <c r="W7" s="43"/>
+      <c r="X7" s="43"/>
+      <c r="Y7" s="43"/>
+      <c r="Z7" s="43"/>
+      <c r="AA7" s="43"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>257</v>
       </c>
@@ -13156,7 +12676,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>262</v>
       </c>
@@ -13194,7 +12714,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>268</v>
       </c>
@@ -13232,7 +12752,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>273</v>
       </c>
@@ -13270,7 +12790,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>277</v>
       </c>
@@ -13308,7 +12828,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>283</v>
       </c>
@@ -13346,7 +12866,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>289</v>
       </c>
@@ -13384,7 +12904,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>294</v>
       </c>
@@ -13422,7 +12942,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>300</v>
       </c>
@@ -31908,8 +31428,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C3:L3"/>
+    <mergeCell ref="R7:AA7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31917,10 +31438,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82FC352-F54F-44E2-863E-F5653510121D}">
-  <dimension ref="A1:Q278"/>
+  <dimension ref="A1:AD282"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B281" sqref="B281:I281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31934,7 +31455,7 @@
     <col min="17" max="17" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1484</v>
       </c>
@@ -31987,7 +31508,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1712</v>
       </c>
@@ -32015,8 +31536,18 @@
       <c r="I2" s="36">
         <v>530</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1713</v>
       </c>
@@ -32044,8 +31575,35 @@
       <c r="I3" s="36">
         <v>815</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="S3" t="s">
+        <v>242</v>
+      </c>
+      <c r="T3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" t="s">
+        <v>4</v>
+      </c>
+      <c r="X3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1714</v>
       </c>
@@ -32073,8 +31631,35 @@
       <c r="I4" s="36">
         <v>878</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="S4" t="s">
+        <v>1215</v>
+      </c>
+      <c r="T4">
+        <v>47</v>
+      </c>
+      <c r="U4" t="s">
+        <v>1216</v>
+      </c>
+      <c r="V4">
+        <v>9533</v>
+      </c>
+      <c r="W4">
+        <v>746</v>
+      </c>
+      <c r="X4">
+        <v>791</v>
+      </c>
+      <c r="Y4">
+        <v>1884</v>
+      </c>
+      <c r="Z4">
+        <v>3541</v>
+      </c>
+      <c r="AA4">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1715</v>
       </c>
@@ -32102,8 +31687,35 @@
       <c r="I5" s="36">
         <v>814</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="S5" t="s">
+        <v>1217</v>
+      </c>
+      <c r="T5">
+        <v>81</v>
+      </c>
+      <c r="U5" t="s">
+        <v>1218</v>
+      </c>
+      <c r="V5">
+        <v>6943</v>
+      </c>
+      <c r="W5">
+        <v>687</v>
+      </c>
+      <c r="X5">
+        <v>794</v>
+      </c>
+      <c r="Y5">
+        <v>1121</v>
+      </c>
+      <c r="Z5">
+        <v>2715</v>
+      </c>
+      <c r="AA5">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1716</v>
       </c>
@@ -32131,8 +31743,35 @@
       <c r="I6" s="36">
         <v>807</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="S6" t="s">
+        <v>1219</v>
+      </c>
+      <c r="T6">
+        <v>235</v>
+      </c>
+      <c r="U6" t="s">
+        <v>1221</v>
+      </c>
+      <c r="V6" t="s">
+        <v>1220</v>
+      </c>
+      <c r="W6">
+        <v>7876</v>
+      </c>
+      <c r="X6">
+        <v>1403</v>
+      </c>
+      <c r="Y6">
+        <v>933</v>
+      </c>
+      <c r="Z6">
+        <v>9587</v>
+      </c>
+      <c r="AA6">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>1717</v>
       </c>
@@ -32160,8 +31799,35 @@
       <c r="I7" s="36">
         <v>415</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="S7" t="s">
+        <v>1222</v>
+      </c>
+      <c r="T7">
+        <v>357</v>
+      </c>
+      <c r="U7" t="s">
+        <v>1224</v>
+      </c>
+      <c r="V7" t="s">
+        <v>1223</v>
+      </c>
+      <c r="W7">
+        <v>6370</v>
+      </c>
+      <c r="X7">
+        <v>1486</v>
+      </c>
+      <c r="Y7">
+        <v>964</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>1225</v>
+      </c>
+      <c r="AA7">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>1718</v>
       </c>
@@ -32190,7 +31856,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>1727</v>
       </c>
@@ -32219,7 +31885,7 @@
         <v>3382</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>1728</v>
       </c>
@@ -32248,7 +31914,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1719</v>
       </c>
@@ -32277,7 +31943,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>1720</v>
       </c>
@@ -32306,7 +31972,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>1721</v>
       </c>
@@ -32335,7 +32001,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>1722</v>
       </c>
@@ -32364,7 +32030,7 @@
         <v>3306</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>1723</v>
       </c>
@@ -32393,7 +32059,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>1724</v>
       </c>
@@ -40021,13 +39687,131 @@
         <v>700</v>
       </c>
     </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A279" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B279" s="36">
+        <v>47</v>
+      </c>
+      <c r="C279" s="36" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D279" s="36">
+        <v>9533</v>
+      </c>
+      <c r="E279" s="36">
+        <v>746</v>
+      </c>
+      <c r="F279" s="36">
+        <v>791</v>
+      </c>
+      <c r="G279" s="36">
+        <v>1884</v>
+      </c>
+      <c r="H279" s="36">
+        <v>3541</v>
+      </c>
+      <c r="I279" s="36">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A280" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B280" s="36">
+        <v>81</v>
+      </c>
+      <c r="C280" s="36" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D280" s="36">
+        <v>6943</v>
+      </c>
+      <c r="E280" s="36">
+        <v>687</v>
+      </c>
+      <c r="F280" s="36">
+        <v>794</v>
+      </c>
+      <c r="G280" s="36">
+        <v>1121</v>
+      </c>
+      <c r="H280" s="36">
+        <v>2715</v>
+      </c>
+      <c r="I280" s="36">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A281" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B281" s="36">
+        <v>235</v>
+      </c>
+      <c r="C281" s="36" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D281" s="36" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E281" s="36">
+        <v>7876</v>
+      </c>
+      <c r="F281" s="36">
+        <v>1403</v>
+      </c>
+      <c r="G281" s="36">
+        <v>933</v>
+      </c>
+      <c r="H281" s="36">
+        <v>9587</v>
+      </c>
+      <c r="I281" s="36">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A282" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B282" s="36">
+        <v>357</v>
+      </c>
+      <c r="C282" s="36" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D282" s="36" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E282" s="36">
+        <v>6370</v>
+      </c>
+      <c r="F282" s="36">
+        <v>1486</v>
+      </c>
+      <c r="G282" s="36">
+        <v>964</v>
+      </c>
+      <c r="H282" s="36" t="s">
+        <v>1225</v>
+      </c>
+      <c r="I282" s="36">
+        <v>614</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="U2:AD2"/>
+  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exporting databases and re-running some sites
</commit_message>
<xml_diff>
--- a/data/new_file_lithiumsites.xlsx
+++ b/data/new_file_lithiumsites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schenker\PycharmProjects\Geothermal_brines\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7542A3D-8749-41BB-B249-9127F1F79654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B767F579-5A54-4E58-84EA-8CD8B3035954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
+    <workbookView minimized="1" xWindow="-83" yWindow="195" windowWidth="14400" windowHeight="7290" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet4!$A$2:$A$282</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet4!$B$2:$B$282</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="1791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4201" uniqueCount="1792">
   <si>
     <t>Site name</t>
   </si>
@@ -5416,6 +5412,9 @@
   </si>
   <si>
     <t>Sal del Los Angeles</t>
+  </si>
+  <si>
+    <t>salar_DLE_spec</t>
   </si>
 </sst>
 </file>
@@ -5568,7 +5567,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5689,8 +5688,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6120,20 +6117,17 @@
   <dimension ref="A1:AL101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z50" sqref="Z50"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14.3984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.1328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.59765625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="8.59765625" style="1" customWidth="1"/>
+    <col min="2" max="7" width="19.46484375" style="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.1328125" style="1"/>
-    <col min="10" max="10" width="11.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.46484375" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.1328125" style="1"/>
     <col min="12" max="12" width="11.265625" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.1328125" style="1" bestFit="1" customWidth="1"/>
@@ -6543,10 +6537,10 @@
         <v>1769</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>1769</v>
+        <v>1791</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>1769</v>
+        <v>1791</v>
       </c>
       <c r="Z5" s="1" t="s">
         <v>1769</v>
@@ -7451,15 +7445,15 @@
         <f>((Sheet2!Y5/1000)/(Sheet1!$Z$13*1000))*100</f>
         <v>0.64557377049180331</v>
       </c>
-      <c r="AD18" s="44"/>
-      <c r="AE18" s="45"/>
-      <c r="AF18" s="45"/>
-      <c r="AG18" s="45"/>
-      <c r="AH18" s="45"/>
-      <c r="AI18" s="45"/>
-      <c r="AJ18" s="45"/>
-      <c r="AK18" s="45"/>
-      <c r="AL18" s="45"/>
+      <c r="AD18"/>
+      <c r="AE18" s="36"/>
+      <c r="AF18" s="36"/>
+      <c r="AG18" s="36"/>
+      <c r="AH18" s="36"/>
+      <c r="AI18" s="36"/>
+      <c r="AJ18" s="36"/>
+      <c r="AK18" s="36"/>
+      <c r="AL18" s="36"/>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
@@ -10107,7 +10101,7 @@
         <v>170</v>
       </c>
       <c r="J71" s="17" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="K71" s="17" t="s">
         <v>170</v>
@@ -10119,7 +10113,7 @@
         <v>170</v>
       </c>
       <c r="N71" s="17" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="O71" s="17" t="s">
         <v>168</v>
@@ -10186,8 +10180,8 @@
       <c r="I72" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="J72" s="17" t="s">
-        <v>156</v>
+      <c r="J72" s="35" t="s">
+        <v>151</v>
       </c>
       <c r="K72" s="35" t="s">
         <v>151</v>
@@ -10199,7 +10193,7 @@
         <v>151</v>
       </c>
       <c r="N72" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O72" s="17" t="s">
         <v>169</v>
@@ -10267,7 +10261,7 @@
         <v>152</v>
       </c>
       <c r="J73" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K73" s="35" t="s">
         <v>152</v>
@@ -10279,7 +10273,7 @@
         <v>152</v>
       </c>
       <c r="N73" s="17" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="O73" s="17" t="s">
         <v>170</v>
@@ -10347,7 +10341,7 @@
         <v>156</v>
       </c>
       <c r="J74" s="17" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="K74" s="35" t="s">
         <v>156</v>
@@ -10359,7 +10353,7 @@
         <v>156</v>
       </c>
       <c r="N74" s="17" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="O74" s="17" t="s">
         <v>171</v>
@@ -10427,7 +10421,7 @@
         <v>154</v>
       </c>
       <c r="J75" s="17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K75" s="35" t="s">
         <v>154</v>
@@ -10439,7 +10433,7 @@
         <v>154</v>
       </c>
       <c r="N75" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O75" s="17" t="s">
         <v>172</v>
@@ -10507,7 +10501,7 @@
         <v>176</v>
       </c>
       <c r="J76" s="17" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="K76" s="35" t="s">
         <v>176</v>
@@ -10519,7 +10513,7 @@
         <v>176</v>
       </c>
       <c r="N76" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O76" s="17" t="s">
         <v>173</v>
@@ -10587,7 +10581,7 @@
         <v>157</v>
       </c>
       <c r="J77" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K77" s="35" t="s">
         <v>157</v>
@@ -10599,7 +10593,7 @@
         <v>157</v>
       </c>
       <c r="N77" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O77" s="17" t="s">
         <v>174</v>
@@ -10667,7 +10661,7 @@
         <v>158</v>
       </c>
       <c r="J78" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K78" s="35" t="s">
         <v>158</v>
@@ -10679,7 +10673,7 @@
         <v>158</v>
       </c>
       <c r="N78" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O78" s="17" t="s">
         <v>157</v>
@@ -10747,7 +10741,7 @@
         <v>159</v>
       </c>
       <c r="J79" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K79" s="35" t="s">
         <v>159</v>
@@ -10759,7 +10753,7 @@
         <v>159</v>
       </c>
       <c r="N79" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O79" s="17" t="s">
         <v>158</v>
@@ -10827,7 +10821,7 @@
         <v>160</v>
       </c>
       <c r="J80" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K80" s="35" t="s">
         <v>160</v>
@@ -10839,7 +10833,7 @@
         <v>160</v>
       </c>
       <c r="N80" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O80" s="17" t="s">
         <v>159</v>
@@ -10907,7 +10901,7 @@
         <v>161</v>
       </c>
       <c r="J81" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K81" s="35" t="s">
         <v>161</v>
@@ -10919,7 +10913,7 @@
         <v>161</v>
       </c>
       <c r="N81" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O81" s="17" t="s">
         <v>160</v>
@@ -10987,7 +10981,7 @@
         <v>162</v>
       </c>
       <c r="J82" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K82" s="35" t="s">
         <v>162</v>
@@ -10998,8 +10992,8 @@
       <c r="M82" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="N82" s="1" t="s">
-        <v>165</v>
+      <c r="N82" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="O82" s="17" t="s">
         <v>161</v>
@@ -11066,8 +11060,8 @@
       <c r="I83" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="J83" s="1" t="s">
-        <v>165</v>
+      <c r="J83" s="17" t="s">
+        <v>163</v>
       </c>
       <c r="K83" s="35" t="s">
         <v>163</v>
@@ -11077,6 +11071,9 @@
       </c>
       <c r="M83" s="17" t="s">
         <v>163</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="O83" s="17" t="s">
         <v>162</v>
@@ -11143,6 +11140,9 @@
       <c r="I84" s="17" t="s">
         <v>164</v>
       </c>
+      <c r="J84" s="17" t="s">
+        <v>164</v>
+      </c>
       <c r="K84" s="35" t="s">
         <v>164</v>
       </c>
@@ -11212,6 +11212,9 @@
         <v>165</v>
       </c>
       <c r="I85" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J85" s="1" t="s">
         <v>165</v>
       </c>
       <c r="K85" s="14" t="s">
@@ -11613,7 +11616,7 @@
       <c r="Q2">
         <v>0.84</v>
       </c>
-      <c r="Y2" s="45">
+      <c r="Y2" s="36">
         <v>235</v>
       </c>
     </row>
@@ -11655,7 +11658,7 @@
       <c r="Q3">
         <v>203.7</v>
       </c>
-      <c r="Y3" s="45">
+      <c r="Y3" s="36">
         <v>38270</v>
       </c>
     </row>
@@ -11697,7 +11700,7 @@
       <c r="Q4">
         <v>105.4</v>
       </c>
-      <c r="Y4" s="45">
+      <c r="Y4" s="36">
         <v>21535</v>
       </c>
     </row>
@@ -11745,7 +11748,7 @@
       <c r="Q5">
         <v>15.7</v>
       </c>
-      <c r="Y5" s="45">
+      <c r="Y5" s="36">
         <v>7876</v>
       </c>
     </row>
@@ -11790,7 +11793,7 @@
       <c r="Q6">
         <v>3.33</v>
       </c>
-      <c r="Y6" s="45">
+      <c r="Y6" s="36">
         <v>1403</v>
       </c>
     </row>
@@ -11841,7 +11844,7 @@
       <c r="Q7">
         <v>16.7</v>
       </c>
-      <c r="Y7" s="45">
+      <c r="Y7" s="36">
         <v>933</v>
       </c>
     </row>
@@ -11883,7 +11886,7 @@
       <c r="Q8">
         <v>21.3</v>
       </c>
-      <c r="Y8" s="45">
+      <c r="Y8" s="36">
         <v>9587</v>
       </c>
     </row>
@@ -11931,7 +11934,7 @@
       <c r="Q9">
         <v>0.7</v>
       </c>
-      <c r="Y9" s="45">
+      <c r="Y9" s="36">
         <v>808</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update IX based technology, DLE - water re-circulation
</commit_message>
<xml_diff>
--- a/data/new_file_lithiumsites.xlsx
+++ b/data/new_file_lithiumsites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schenker\PycharmProjects\Geothermal_brines\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67B01FF-BFAC-4EC9-85E7-4296C940ED55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EE699A-6374-4536-8FB2-AC22EC5BAFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4201" uniqueCount="1791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4201" uniqueCount="1790">
   <si>
     <t>Site name</t>
   </si>
@@ -5409,9 +5409,6 @@
   </si>
   <si>
     <t>Sal del Los Angeles</t>
-  </si>
-  <si>
-    <t>salar_DLE_spec</t>
   </si>
 </sst>
 </file>
@@ -6114,8 +6111,8 @@
   <dimension ref="A1:AL101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S15" sqref="S15"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6139,7 +6136,9 @@
     <col min="24" max="24" width="13.86328125" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.1328125" style="1"/>
     <col min="26" max="26" width="15.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.1328125" style="1"/>
+    <col min="27" max="27" width="9.1328125" style="1"/>
+    <col min="28" max="28" width="15.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.45">
@@ -6534,10 +6533,10 @@
         <v>1769</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>1790</v>
+        <v>1769</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>1790</v>
+        <v>1769</v>
       </c>
       <c r="Z5" s="1" t="s">
         <v>1769</v>
@@ -9210,7 +9209,7 @@
         <v>2030000</v>
       </c>
       <c r="D49" s="10">
-        <v>70000000</v>
+        <v>202500000</v>
       </c>
       <c r="E49" s="11">
         <v>12605000</v>
@@ -9357,8 +9356,9 @@
       <c r="C52" s="1">
         <v>80</v>
       </c>
-      <c r="D52" s="1">
-        <v>477.4</v>
+      <c r="D52" s="13">
+        <f>477.4* (D49/70000000)</f>
+        <v>1381.05</v>
       </c>
       <c r="E52" s="1">
         <v>180</v>

</xml_diff>

<commit_message>
Improvements + automatized LSA
</commit_message>
<xml_diff>
--- a/data/new_file_lithiumsites.xlsx
+++ b/data/new_file_lithiumsites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schenker\PycharmProjects\Geothermal_brines\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003BCD7B-D558-46BE-97F0-D895C48B0E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75333166-859D-4566-9B37-94901846E8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39690" yWindow="2715" windowWidth="21600" windowHeight="11025" tabRatio="704" activeTab="3" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5406" uniqueCount="1790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5407" uniqueCount="1790">
   <si>
     <t>Site name</t>
   </si>
@@ -5382,46 +5382,48 @@
     <t>Reserves Development</t>
   </si>
   <si>
+    <t>Advanced exploration</t>
+  </si>
+  <si>
+    <t>sum_impurities</t>
+  </si>
+  <si>
+    <t>Feasibility Started</t>
+  </si>
+  <si>
+    <t>Ang_1</t>
+  </si>
+  <si>
+    <t>Ang_2</t>
+  </si>
+  <si>
+    <t>Ang_3</t>
+  </si>
+  <si>
+    <t>Ang_4</t>
+  </si>
+  <si>
+    <t>Sal del Los Angeles</t>
+  </si>
+  <si>
     <t>Commissioning</t>
   </si>
   <si>
     <t>Preproduction</t>
-  </si>
-  <si>
-    <t>Advanced exploration</t>
-  </si>
-  <si>
-    <t>sum_impurities</t>
-  </si>
-  <si>
-    <t>Feasibility Started</t>
-  </si>
-  <si>
-    <t>Ang_1</t>
-  </si>
-  <si>
-    <t>Ang_2</t>
-  </si>
-  <si>
-    <t>Ang_3</t>
-  </si>
-  <si>
-    <t>Ang_4</t>
-  </si>
-  <si>
-    <t>Sal del Los Angeles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -5503,7 +5505,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5518,9 +5520,6 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5544,16 +5543,9 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5573,6 +5565,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5683,21 +5682,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B9A88C4-4092-4296-A064-E411E5F9DB7E}" name="Table132" displayName="Table132" ref="A1:Q282" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B9A88C4-4092-4296-A064-E411E5F9DB7E}" name="Table132" displayName="Table132" ref="A1:Q282" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A1:Q282" xr:uid="{7B9A88C4-4092-4296-A064-E411E5F9DB7E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q278">
     <sortCondition ref="A1:A278"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{9717A187-DC4A-4D4D-B924-EFA8E9056C8F}" name="site_identifier"/>
-    <tableColumn id="2" xr3:uid="{30D97636-695E-4B51-81F4-85E8CD32E753}" name="ini_Li" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{F4AA01F3-56ED-4DB2-B6E2-C8D9F4EA7143}" name="ini_Cl" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{12ADB1B1-F079-49D5-8671-95545F1FBBE4}" name="ini_Na" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{B55ADEDE-1F3E-4815-AD08-FC0E8822BD14}" name="ini_K" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{B94FD87B-7996-40B0-99A6-5546778F3D39}" name="ini_Ca" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{B68E1AE0-DEF9-4666-B308-5CF5DDC1A85F}" name="ini_Mg" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{C2AD89A4-F2F6-42AB-9C4F-63947F91330C}" name="ini_SO4" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{DA1EFC8D-830C-4752-9D44-72FB2BB52671}" name="ini_B" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{30D97636-695E-4B51-81F4-85E8CD32E753}" name="ini_Li" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{F4AA01F3-56ED-4DB2-B6E2-C8D9F4EA7143}" name="ini_Cl" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{12ADB1B1-F079-49D5-8671-95545F1FBBE4}" name="ini_Na" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{B55ADEDE-1F3E-4815-AD08-FC0E8822BD14}" name="ini_K" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{B94FD87B-7996-40B0-99A6-5546778F3D39}" name="ini_Ca" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{B68E1AE0-DEF9-4666-B308-5CF5DDC1A85F}" name="ini_Mg" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{C2AD89A4-F2F6-42AB-9C4F-63947F91330C}" name="ini_SO4" dataDxfId="10" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{DA1EFC8D-830C-4752-9D44-72FB2BB52671}" name="ini_B" dataDxfId="9"/>
     <tableColumn id="10" xr3:uid="{E9B7CCC2-1469-4792-847A-CE7AF32BDE06}" name="ini_Si"/>
     <tableColumn id="11" xr3:uid="{0D927DBA-9975-4C9A-A113-4110038C1258}" name="ini_As"/>
     <tableColumn id="12" xr3:uid="{3875EF4C-7AAE-43E1-BDD6-64411C09E212}" name="ini_Mn"/>
@@ -5712,21 +5711,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{03EACCB9-7AFB-4480-95EC-51BD3D1FC6C3}" name="Table13" displayName="Table13" ref="A1:Q282" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{03EACCB9-7AFB-4480-95EC-51BD3D1FC6C3}" name="Table13" displayName="Table13" ref="A1:Q282" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:Q282" xr:uid="{03EACCB9-7AFB-4480-95EC-51BD3D1FC6C3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q278">
     <sortCondition ref="A1:A278"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{334CC8CD-A1BC-4783-803C-5CB48F4A0BAF}" name="site_identifier"/>
-    <tableColumn id="2" xr3:uid="{50C70ABA-B313-46F2-BCF3-2EF78ACC0CE8}" name="ini_Li" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{399952D8-6349-471A-9767-328C485D5A7B}" name="ini_Cl" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{57172103-0204-4271-973D-683613E49269}" name="ini_Na" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{D878154D-AFEF-4F51-9749-B4E525F22EF9}" name="ini_K" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{B996DEE3-7FFC-48A1-AD9F-12704E8C0457}" name="ini_Ca" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{A67DFC72-A7E0-4488-B4C1-2F1400BEA40F}" name="ini_Mg" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{BBDD3F35-6B04-453C-81A9-10C6537F02EF}" name="ini_SO4" dataDxfId="10" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{4503D5A4-FA19-42DF-AE09-08492D52999D}" name="ini_B" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{50C70ABA-B313-46F2-BCF3-2EF78ACC0CE8}" name="ini_Li" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{399952D8-6349-471A-9767-328C485D5A7B}" name="ini_Cl" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{57172103-0204-4271-973D-683613E49269}" name="ini_Na" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{D878154D-AFEF-4F51-9749-B4E525F22EF9}" name="ini_K" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{B996DEE3-7FFC-48A1-AD9F-12704E8C0457}" name="ini_Ca" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{A67DFC72-A7E0-4488-B4C1-2F1400BEA40F}" name="ini_Mg" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{BBDD3F35-6B04-453C-81A9-10C6537F02EF}" name="ini_SO4" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{4503D5A4-FA19-42DF-AE09-08492D52999D}" name="ini_B" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{4164B84D-CD01-416F-8025-8D3AF02257F7}" name="ini_Si"/>
     <tableColumn id="11" xr3:uid="{8F628721-E3C2-40E9-8705-050550634F57}" name="ini_As"/>
     <tableColumn id="12" xr3:uid="{7F059D6F-B7E8-4104-B9B3-55FD35576903}" name="ini_Mn"/>
@@ -6075,983 +6074,982 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5319587E-5250-4C3E-BD3D-6C0619F44C22}">
   <dimension ref="A1:AL101"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.3984375" style="10" customWidth="1"/>
-    <col min="2" max="7" width="19.3984375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="12" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.1328125" style="11"/>
-    <col min="10" max="10" width="23.3984375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="9.1328125" style="11"/>
-    <col min="12" max="12" width="11.265625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="13.1328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1328125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.1328125" style="11" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="27.73046875" style="11" customWidth="1"/>
-    <col min="17" max="18" width="9.1328125" style="11"/>
-    <col min="19" max="19" width="27.265625" style="11" customWidth="1"/>
-    <col min="20" max="20" width="13.1328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.3984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.1328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.1328125" style="11"/>
-    <col min="26" max="26" width="15.265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.1328125" style="11"/>
-    <col min="28" max="28" width="15.265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.1328125" style="11"/>
+    <col min="1" max="1" width="14.3984375" style="9" customWidth="1"/>
+    <col min="2" max="7" width="19.3984375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="12" style="10" customWidth="1"/>
+    <col min="9" max="9" width="9.1328125" style="10"/>
+    <col min="10" max="10" width="23.3984375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="9.1328125" style="10"/>
+    <col min="12" max="12" width="11.265625" style="10" customWidth="1"/>
+    <col min="13" max="15" width="21.53125" style="10" customWidth="1"/>
+    <col min="16" max="16" width="27.73046875" style="10" customWidth="1"/>
+    <col min="17" max="18" width="9.1328125" style="10"/>
+    <col min="19" max="19" width="27.265625" style="10" customWidth="1"/>
+    <col min="20" max="20" width="13.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.1328125" style="10"/>
+    <col min="28" max="28" width="15.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.1328125" style="10"/>
+    <col min="30" max="30" width="14.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.1328125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27" t="s">
+    <row r="1" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="R1" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="S1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="T1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Y1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="Z1" s="23" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="T2" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="U2" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="V2" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="W2" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="X2" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="Y2" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="Z2" s="10" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="11" t="str">
-        <f>G3</f>
-        <v>salar</v>
-      </c>
-      <c r="N3" s="11" t="s">
+      <c r="M3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="N3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="O3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="P3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="Q3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="R3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="S3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="T3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="U3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="V3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="W3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="X3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="Y3" s="29" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A4" s="10" t="s">
+      <c r="Z3" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="29" t="s">
         <v>1772</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="29" t="s">
         <v>1776</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="29" t="s">
         <v>1773</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="29" t="s">
         <v>1774</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="29" t="s">
         <v>1774</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="29" t="s">
         <v>1774</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="29" t="s">
         <v>1775</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="29" t="s">
         <v>1776</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="29" t="s">
         <v>1773</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="29" t="s">
         <v>1777</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="29" t="s">
+        <v>1780</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>1775</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>1774</v>
+      </c>
+      <c r="N4" s="29" t="s">
+        <v>1776</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>1778</v>
+      </c>
+      <c r="P4" s="29" t="s">
+        <v>1777</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>1776</v>
+      </c>
+      <c r="R4" s="29" t="s">
+        <v>1777</v>
+      </c>
+      <c r="S4" s="29" t="s">
+        <v>1779</v>
+      </c>
+      <c r="T4" s="29" t="s">
+        <v>1778</v>
+      </c>
+      <c r="U4" s="29" t="s">
+        <v>1776</v>
+      </c>
+      <c r="V4" s="29" t="s">
+        <v>1774</v>
+      </c>
+      <c r="W4" s="29" t="s">
         <v>1782</v>
       </c>
-      <c r="L4" s="11" t="s">
-        <v>1775</v>
-      </c>
-      <c r="M4" s="11" t="s">
+      <c r="X4" s="29" t="s">
         <v>1774</v>
       </c>
-      <c r="N4" s="11" t="s">
-        <v>1776</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>1778</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>1777</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>1776</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>1777</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>1779</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>1778</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>1776</v>
-      </c>
-      <c r="V4" s="11" t="s">
-        <v>1774</v>
-      </c>
-      <c r="W4" s="11" t="s">
-        <v>1784</v>
-      </c>
-      <c r="X4" s="11" t="s">
-        <v>1774</v>
-      </c>
-      <c r="Y4" s="11" t="s">
-        <v>1780</v>
-      </c>
-      <c r="Z4" s="11" t="s">
-        <v>1781</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A5" s="10" t="s">
+      <c r="Y4" s="29" t="s">
+        <v>1788</v>
+      </c>
+      <c r="Z4" s="29" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="29" t="s">
         <v>1767</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="29" t="s">
         <v>1768</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="29" t="s">
         <v>1768</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="29" t="s">
         <v>1770</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="29" t="s">
         <v>1771</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="29" t="s">
         <v>1770</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="29" t="s">
         <v>1770</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="29" t="s">
         <v>1770</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="29" t="s">
         <v>1770</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="29" t="s">
         <v>1770</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="Q5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="R5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="S5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="T5" s="29" t="s">
         <v>1770</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="U5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="V5" s="11" t="s">
+      <c r="V5" s="29" t="s">
         <v>1771</v>
       </c>
-      <c r="W5" s="11" t="s">
+      <c r="W5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="X5" s="11" t="s">
+      <c r="X5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="Y5" s="11" t="s">
+      <c r="Y5" s="29" t="s">
         <v>1769</v>
       </c>
-      <c r="Z5" s="11" t="s">
+      <c r="Z5" s="29" t="s">
         <v>1769</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="11" t="str">
+      <c r="M6" s="10" t="str">
         <f>G6</f>
         <v>AR</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="P6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="Q6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="S6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="T6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="U6" s="10" t="s">
         <v>1764</v>
       </c>
-      <c r="V6" s="11" t="s">
+      <c r="V6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="W6" s="11" t="s">
+      <c r="W6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="X6" s="11" t="s">
+      <c r="X6" s="10" t="s">
         <v>1766</v>
       </c>
-      <c r="Y6" s="11" t="s">
+      <c r="Y6" s="10" t="s">
         <v>1766</v>
       </c>
-      <c r="Z6" s="11" t="s">
+      <c r="Z6" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>-71</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>143</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>2300</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>3900</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>3000</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>4000</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>4100</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <v>3718</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <v>3480</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>3660</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <v>3630</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="10">
         <f>G7</f>
         <v>4000</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="10">
         <f>G7</f>
         <v>4000</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="10">
         <v>3780</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="10">
         <v>3330</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="Q7" s="10">
         <v>3820</v>
       </c>
-      <c r="R7" s="11">
+      <c r="R7" s="10">
         <v>3760</v>
       </c>
-      <c r="S7" s="11">
+      <c r="S7" s="10">
         <v>3414</v>
       </c>
-      <c r="T7" s="11">
+      <c r="T7" s="10">
         <v>3750</v>
       </c>
-      <c r="U7" s="11">
+      <c r="U7" s="10">
         <v>3653</v>
       </c>
-      <c r="V7" s="11">
+      <c r="V7" s="10">
         <v>1544</v>
       </c>
-      <c r="W7" s="11">
+      <c r="W7" s="10">
         <v>3000</v>
       </c>
-      <c r="X7" s="11">
+      <c r="X7" s="10">
         <v>2670</v>
       </c>
-      <c r="Y7" s="11">
+      <c r="Y7" s="10">
         <v>2700</v>
       </c>
-      <c r="Z7" s="11">
+      <c r="Z7" s="10">
         <v>4060</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>-115.57814</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>7.9751099999999999</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>-68.32159</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>-66.7</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>-66.790670000000006</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>-66.981870000000001</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="12">
         <v>-68.665130000000005</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="12">
         <v>-67.12</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="12">
         <v>-67.709720000000004</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <v>-68.14443</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="12">
         <v>-67.124110000000002</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="12">
         <v>-67.048779999999994</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="12">
         <v>-66.947149999999993</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="12">
         <v>-66.704589999999996</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="12">
         <v>-67.462999999999994</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="12">
         <v>-66.816280000000006</v>
       </c>
-      <c r="R8" s="13">
+      <c r="R8" s="12">
         <v>-66.817809999999994</v>
       </c>
-      <c r="S8" s="13">
+      <c r="S8" s="12">
         <v>-65.946389999999994</v>
       </c>
-      <c r="T8" s="13">
+      <c r="T8" s="12">
         <v>-69.071663999999998</v>
       </c>
-      <c r="U8" s="13">
+      <c r="U8" s="12">
         <v>-67.378029999999995</v>
       </c>
-      <c r="V8" s="13">
+      <c r="V8" s="12">
         <v>-117.57931000000001</v>
       </c>
-      <c r="W8" s="13">
+      <c r="W8" s="12">
         <v>-67.428989999999999</v>
       </c>
-      <c r="X8" s="13">
+      <c r="X8" s="12">
         <v>95.240380000000002</v>
       </c>
-      <c r="Y8" s="13">
+      <c r="Y8" s="12">
         <v>91.483860000000007</v>
       </c>
-      <c r="Z8" s="13">
+      <c r="Z8" s="12">
         <v>-66.748329999999996</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>33.177570000000003</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <v>48.65578</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <v>-23.641819999999999</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>-23.45</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <v>-23.757380000000001</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <v>-25.225560000000002</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="12">
         <v>-27.364129999999999</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="12">
         <v>-24.057500000000001</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="12">
         <v>-24.770140000000001</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="12">
         <v>-25.006049999999998</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="12">
         <v>-25.036719999999999</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="12">
         <v>-25.392700000000001</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="12">
         <v>-25.345320000000001</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="12">
         <v>-24.57086</v>
       </c>
-      <c r="P9" s="13">
+      <c r="P9" s="12">
         <v>-25.248000000000001</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="12">
         <v>-25.090769999999999</v>
       </c>
-      <c r="R9" s="13">
+      <c r="R9" s="12">
         <v>-24.698969999999999</v>
       </c>
-      <c r="S9" s="13">
+      <c r="S9" s="12">
         <v>-23.728560000000002</v>
       </c>
-      <c r="T9" s="13">
+      <c r="T9" s="12">
         <v>-26.877735999999999</v>
       </c>
-      <c r="U9" s="13">
+      <c r="U9" s="12">
         <v>-20.542850000000001</v>
       </c>
-      <c r="V9" s="13">
+      <c r="V9" s="12">
         <v>37.775440000000003</v>
       </c>
-      <c r="W9" s="13">
+      <c r="W9" s="12">
         <v>-26.498830000000002</v>
       </c>
-      <c r="X9" s="13">
+      <c r="X9" s="12">
         <v>36.78454</v>
       </c>
-      <c r="Y9" s="13">
+      <c r="Y9" s="12">
         <v>38.540610000000001</v>
       </c>
-      <c r="Z9" s="13">
+      <c r="Z9" s="12">
         <v>-25.244720000000001</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>22</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>15</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>16.8</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>8.24</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <v>5.2</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>4</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <v>6.5</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="10">
         <f>5.2</f>
         <v>5.2</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N10" s="10">
         <f>G10</f>
         <v>5.2</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="10">
         <v>6.3</v>
       </c>
-      <c r="S10" s="13"/>
-      <c r="T10" s="11">
+      <c r="S10" s="12"/>
+      <c r="T10" s="10">
         <v>5.5</v>
       </c>
-      <c r="U10" s="11">
+      <c r="U10" s="10">
         <v>7.8</v>
       </c>
-      <c r="V10" s="11">
+      <c r="V10" s="10">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="11">
-        <v>0</v>
-      </c>
-      <c r="D11" s="11">
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
         <v>1.44</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <v>1.246</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>1.27</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <v>1.1060000000000001</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>1.788</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>1.2330000000000001</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <v>2.044</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="10">
         <f>G11</f>
         <v>1.1060000000000001</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="10">
         <f>G11</f>
         <v>1.1060000000000001</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="10">
         <v>1.2</v>
       </c>
-      <c r="T11" s="11">
+      <c r="T11" s="10">
         <f>D11</f>
         <v>1.44</v>
       </c>
-      <c r="U11" s="11">
+      <c r="U11" s="10">
         <v>1.3180000000000001</v>
       </c>
-      <c r="V11" s="11">
+      <c r="V11" s="10">
         <v>1.425</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>100</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>100</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>99.5</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>86.8</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>89</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <v>86.4</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>94.9</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="10">
         <f>G12</f>
         <v>86.4</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="10">
         <f>G12</f>
         <v>86.4</v>
       </c>
-      <c r="V12" s="11">
+      <c r="V12" s="10">
         <v>94.92</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>1.1299999999999999</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>1.1299999999999999</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>1.2230000000000001</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>1.2110000000000001</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <v>1.22</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <v>1.206</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>1.2370000000000001</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>1.22</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="10">
         <v>1.22</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="10">
         <v>1.22</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="10">
         <v>1.2</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="10">
         <f>G13</f>
         <v>1.206</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N13" s="10">
         <f>G13</f>
         <v>1.206</v>
       </c>
-      <c r="O13" s="11">
+      <c r="O13" s="10">
         <v>1.22</v>
       </c>
-      <c r="P13" s="11">
+      <c r="P13" s="10">
         <v>1.22</v>
       </c>
-      <c r="Q13" s="11">
+      <c r="Q13" s="10">
         <v>1.22</v>
       </c>
-      <c r="R13" s="11">
+      <c r="R13" s="10">
         <v>1.22</v>
       </c>
-      <c r="S13" s="11">
+      <c r="S13" s="10">
         <v>1.22</v>
       </c>
-      <c r="T13" s="11">
+      <c r="T13" s="10">
         <v>1.2</v>
       </c>
-      <c r="U13" s="11">
+      <c r="U13" s="10">
         <v>1.2</v>
       </c>
-      <c r="V13" s="11">
+      <c r="V13" s="10">
         <v>1.2</v>
       </c>
-      <c r="X13" s="11">
+      <c r="X13" s="10">
         <v>1.349</v>
       </c>
-      <c r="Y13" s="11">
+      <c r="Y13" s="10">
         <v>1.349</v>
       </c>
-      <c r="Z13" s="11">
+      <c r="Z13" s="10">
         <v>1.22</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="8"/>
@@ -7077,7 +7075,7 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>193</v>
       </c>
       <c r="B15" s="8">
@@ -7109,7 +7107,7 @@
       <c r="J15" s="7">
         <v>2.60655737704918E-2</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="13">
         <f>((Sheet2!E2/1000)/(Sheet1!$K$13*1000))*100</f>
         <v>3.4426229508196717E-2</v>
       </c>
@@ -7129,7 +7127,7 @@
         <f>((Sheet2!J2/1000)/(Sheet1!$O$13*1000))*100</f>
         <v>3.5573770491803276E-2</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="13">
         <f>((Sheet2!K2/1000)/(Sheet1!$P$13*1000))*100</f>
         <v>2.5491803278688527E-2</v>
       </c>
@@ -7149,20 +7147,20 @@
         <f>((Sheet2!P2/1000)/(Sheet1!$P$13*1000))*100</f>
         <v>9.1967213114754101E-2</v>
       </c>
-      <c r="U15" s="15">
+      <c r="U15" s="14">
         <f>(Sheet2!Q2/(1000*Sheet1!$U$13))*100</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="V15" s="11">
+      <c r="V15" s="10">
         <v>0.02</v>
       </c>
-      <c r="W15" s="11">
+      <c r="W15" s="10">
         <v>0.02</v>
       </c>
-      <c r="X15" s="11">
+      <c r="X15" s="10">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="Y15" s="11">
+      <c r="Y15" s="10">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="Z15" s="8">
@@ -7171,7 +7169,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>194</v>
       </c>
       <c r="B16" s="8">
@@ -7214,7 +7212,7 @@
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
-      <c r="P16" s="14">
+      <c r="P16" s="13">
         <f>((Sheet2!K3/1000)/(Sheet1!$P$13*1000))*100</f>
         <v>7.2295901639344251</v>
       </c>
@@ -7238,7 +7236,7 @@
         <f>(Sheet2!Q3/(1000*Sheet1!$U$13))*100</f>
         <v>16.974999999999998</v>
       </c>
-      <c r="V16" s="11">
+      <c r="V16" s="10">
         <v>10.06</v>
       </c>
       <c r="Z16" s="8">
@@ -7247,7 +7245,7 @@
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>195</v>
       </c>
       <c r="B17" s="8">
@@ -7290,7 +7288,7 @@
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
-      <c r="P17" s="14">
+      <c r="P17" s="13">
         <f>((Sheet2!K4/1000)/(Sheet1!$P$13*1000))*100</f>
         <v>4.5713114754098365</v>
       </c>
@@ -7314,7 +7312,7 @@
         <f>(Sheet2!Q4/(1000*Sheet1!$U$13))*100</f>
         <v>8.7833333333333332</v>
       </c>
-      <c r="V17" s="11">
+      <c r="V17" s="10">
         <v>6.2</v>
       </c>
       <c r="Z17" s="8">
@@ -7323,7 +7321,7 @@
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>196</v>
       </c>
       <c r="B18" s="8">
@@ -7372,7 +7370,7 @@
         <f>((Sheet2!J5/1000)/(Sheet1!$O$13*1000))*100</f>
         <v>0.37680327868852465</v>
       </c>
-      <c r="P18" s="14">
+      <c r="P18" s="13">
         <f>((Sheet2!K5/1000)/(Sheet1!$P$13*1000))*100</f>
         <v>6.6147540983606562E-2</v>
       </c>
@@ -7396,14 +7394,14 @@
         <f>(Sheet2!Q5/(1000*Sheet1!$U$13))*100</f>
         <v>1.3083333333333331</v>
       </c>
-      <c r="V18" s="11">
+      <c r="V18" s="10">
         <v>0.8</v>
       </c>
       <c r="Z18" s="8">
         <f>((Sheet2!Y5/1000)/(Sheet1!$Z$13*1000))*100</f>
         <v>0.64557377049180331</v>
       </c>
-      <c r="AD18" s="16"/>
+      <c r="AD18" s="15"/>
       <c r="AE18" s="7"/>
       <c r="AF18" s="7"/>
       <c r="AG18" s="7"/>
@@ -7414,7 +7412,7 @@
       <c r="AL18" s="7"/>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>197</v>
       </c>
       <c r="B19" s="8">
@@ -7460,7 +7458,7 @@
       </c>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
-      <c r="P19" s="14">
+      <c r="P19" s="13">
         <f>((Sheet2!K6/1000)/(Sheet1!$P$13*1000))*100</f>
         <v>4.3852459016393446E-2</v>
       </c>
@@ -7484,7 +7482,7 @@
         <f>(Sheet2!Q6/(1000*Sheet1!$U$13))*100</f>
         <v>0.27750000000000002</v>
       </c>
-      <c r="V19" s="11">
+      <c r="V19" s="10">
         <v>0.71</v>
       </c>
       <c r="Z19" s="8">
@@ -7493,7 +7491,7 @@
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>198</v>
       </c>
       <c r="B20" s="8">
@@ -7545,7 +7543,7 @@
         <f>((Sheet2!J7/1000)/(Sheet1!$O$13*1000))*100</f>
         <v>0.25868852459016395</v>
       </c>
-      <c r="P20" s="14">
+      <c r="P20" s="13">
         <f>((Sheet2!K7/1000)/(Sheet1!$P$13*1000))*100</f>
         <v>6.6885245901639342E-2</v>
       </c>
@@ -7569,7 +7567,7 @@
         <f>(Sheet2!Q7/(1000*Sheet1!$U$13))*100</f>
         <v>1.3916666666666666</v>
       </c>
-      <c r="V20" s="11">
+      <c r="V20" s="10">
         <v>0.02</v>
       </c>
       <c r="Z20" s="8">
@@ -7578,7 +7576,7 @@
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>199</v>
       </c>
       <c r="B21" s="8">
@@ -7624,7 +7622,7 @@
         <v>0.89929999999999999</v>
       </c>
       <c r="O21" s="8"/>
-      <c r="P21" s="14">
+      <c r="P21" s="13">
         <f>((Sheet2!K8/1000)/(Sheet1!$P$13*1000))*100</f>
         <v>0.64057377049180331</v>
       </c>
@@ -7648,7 +7646,7 @@
         <f>(Sheet2!Q8/(1000*Sheet1!$U$13))*100</f>
         <v>1.7750000000000001</v>
       </c>
-      <c r="V21" s="11">
+      <c r="V21" s="10">
         <v>0</v>
       </c>
       <c r="Z21" s="8">
@@ -7657,7 +7655,7 @@
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>200</v>
       </c>
       <c r="B22" s="8">
@@ -7706,7 +7704,7 @@
         <f>((Sheet2!J9/1000)/(Sheet1!$O$13*1000))*100</f>
         <v>6.5245901639344267E-2</v>
       </c>
-      <c r="P22" s="14">
+      <c r="P22" s="13">
         <f>((Sheet2!K9/1000)/(Sheet1!$P$13*1000))*100</f>
         <v>7.1967213114754097E-2</v>
       </c>
@@ -7730,7 +7728,7 @@
         <f>(Sheet2!Q9/(1000*Sheet1!$U$13))*100</f>
         <v>5.8333333333333327E-2</v>
       </c>
-      <c r="V22" s="11">
+      <c r="V22" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="Z22" s="8">
@@ -7739,7 +7737,7 @@
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>201</v>
       </c>
       <c r="B23" s="8">
@@ -7748,7 +7746,7 @@
       <c r="C23" s="8">
         <v>5.9469026548672572E-3</v>
       </c>
-      <c r="D23" s="17"/>
+      <c r="D23" s="16"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
@@ -7766,13 +7764,13 @@
       <c r="S23" s="8"/>
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
-      <c r="V23" s="11">
+      <c r="V23" s="10">
         <v>0</v>
       </c>
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>202</v>
       </c>
       <c r="B24" s="8">
@@ -7781,7 +7779,7 @@
       <c r="C24" s="8">
         <v>1.7964601769911506E-3</v>
       </c>
-      <c r="D24" s="17"/>
+      <c r="D24" s="16"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
@@ -7799,13 +7797,13 @@
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8"/>
-      <c r="V24" s="11">
+      <c r="V24" s="10">
         <v>0</v>
       </c>
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>203</v>
       </c>
       <c r="B25" s="8">
@@ -7814,7 +7812,7 @@
       <c r="C25" s="8">
         <v>2.168141592920354E-3</v>
       </c>
-      <c r="D25" s="17"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -7832,13 +7830,13 @@
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
-      <c r="V25" s="11">
+      <c r="V25" s="10">
         <v>0</v>
       </c>
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>204</v>
       </c>
       <c r="B26" s="8">
@@ -7847,7 +7845,7 @@
       <c r="C26" s="8">
         <v>3.3097345132743362E-3</v>
       </c>
-      <c r="D26" s="17"/>
+      <c r="D26" s="16"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
@@ -7865,13 +7863,13 @@
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8"/>
-      <c r="V26" s="11">
+      <c r="V26" s="10">
         <v>0</v>
       </c>
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>205</v>
       </c>
       <c r="B27" s="8">
@@ -7880,7 +7878,7 @@
       <c r="C27" s="8">
         <v>4.6017699115044256E-4</v>
       </c>
-      <c r="D27" s="17"/>
+      <c r="D27" s="16"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -7898,13 +7896,13 @@
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
       <c r="U27" s="8"/>
-      <c r="V27" s="11">
+      <c r="V27" s="10">
         <v>0</v>
       </c>
       <c r="Z27" s="8"/>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>206</v>
       </c>
       <c r="B28" s="8">
@@ -7913,7 +7911,7 @@
       <c r="C28" s="8">
         <v>2.4424778761061947E-2</v>
       </c>
-      <c r="D28" s="17"/>
+      <c r="D28" s="16"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
@@ -7931,13 +7929,13 @@
       <c r="S28" s="8"/>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
-      <c r="V28" s="11">
+      <c r="V28" s="10">
         <v>0</v>
       </c>
       <c r="Z28" s="8"/>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="9" t="s">
         <v>1762</v>
       </c>
       <c r="B29" s="8">
@@ -7946,7 +7944,7 @@
       <c r="C29" s="8">
         <v>1.2743362831858409E-3</v>
       </c>
-      <c r="D29" s="17"/>
+      <c r="D29" s="16"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -7964,13 +7962,13 @@
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
       <c r="U29" s="8"/>
-      <c r="V29" s="11">
+      <c r="V29" s="10">
         <v>0</v>
       </c>
       <c r="Z29" s="8"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="9" t="s">
         <v>207</v>
       </c>
       <c r="B30" s="8">
@@ -8039,7 +8037,7 @@
         <f>100-SUM(U15:U29)</f>
         <v>69.360833333333332</v>
       </c>
-      <c r="V30" s="11">
+      <c r="V30" s="10">
         <f>100 - SUM(V15:V29)</f>
         <v>82.185000000000002</v>
       </c>
@@ -8049,113 +8047,113 @@
       </c>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31" s="10">
         <v>1.1299999999999999</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="10">
         <v>1.1299999999999999</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="10">
         <v>1.333</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="10">
         <v>1.333</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="10">
         <v>1.333</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="10">
         <v>1.333</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="10">
         <v>1.4330000000000001</v>
       </c>
-      <c r="I31" s="11">
+      <c r="I31" s="10">
         <f>I13</f>
         <v>1.22</v>
       </c>
-      <c r="J31" s="11">
+      <c r="J31" s="10">
         <f>J13</f>
         <v>1.22</v>
       </c>
-      <c r="K31" s="11">
+      <c r="K31" s="10">
         <f>K13</f>
         <v>1.22</v>
       </c>
-      <c r="L31" s="11">
+      <c r="L31" s="10">
         <f>L13</f>
         <v>1.2</v>
       </c>
-      <c r="M31" s="11">
+      <c r="M31" s="10">
         <f>M13</f>
         <v>1.206</v>
       </c>
-      <c r="N31" s="11">
+      <c r="N31" s="10">
         <v>1.333</v>
       </c>
-      <c r="O31" s="11">
+      <c r="O31" s="10">
         <v>1.33</v>
       </c>
-      <c r="P31" s="11">
+      <c r="P31" s="10">
         <f>P13</f>
         <v>1.22</v>
       </c>
-      <c r="Q31" s="11">
+      <c r="Q31" s="10">
         <f t="shared" ref="Q31:S31" si="1">Q13</f>
         <v>1.22</v>
       </c>
-      <c r="R31" s="11">
+      <c r="R31" s="10">
         <f t="shared" si="1"/>
         <v>1.22</v>
       </c>
-      <c r="S31" s="11">
+      <c r="S31" s="10">
         <f t="shared" si="1"/>
         <v>1.22</v>
       </c>
-      <c r="U31" s="11">
+      <c r="U31" s="10">
         <f>U13</f>
         <v>1.2</v>
       </c>
-      <c r="V31" s="11">
+      <c r="V31" s="10">
         <v>1.333</v>
       </c>
-      <c r="X31" s="11">
+      <c r="X31" s="10">
         <v>1.349</v>
       </c>
-      <c r="Y31" s="11">
+      <c r="Y31" s="10">
         <v>1.349</v>
       </c>
-      <c r="Z31" s="11">
+      <c r="Z31" s="10">
         <v>1.22</v>
       </c>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.45">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="P32" s="11">
+      <c r="P32" s="10">
         <f t="shared" ref="P32:S45" si="2">P14</f>
         <v>0</v>
       </c>
-      <c r="Q32" s="11">
+      <c r="Q32" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R32" s="11">
+      <c r="R32" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S32" s="11">
+      <c r="S32" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z32" s="8"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="9" t="s">
         <v>208</v>
       </c>
       <c r="B33" s="8">
@@ -8206,19 +8204,19 @@
       <c r="O33" s="8">
         <v>3</v>
       </c>
-      <c r="P33" s="11">
+      <c r="P33" s="10">
         <f t="shared" si="2"/>
         <v>2.5491803278688527E-2</v>
       </c>
-      <c r="Q33" s="11">
+      <c r="Q33" s="10">
         <f t="shared" si="2"/>
         <v>3.0901639344262294E-2</v>
       </c>
-      <c r="R33" s="11">
+      <c r="R33" s="10">
         <f t="shared" si="2"/>
         <v>1.6967213114754097E-2</v>
       </c>
-      <c r="S33" s="11">
+      <c r="S33" s="10">
         <f t="shared" si="2"/>
         <v>2.2131147540983609E-2</v>
       </c>
@@ -8229,16 +8227,16 @@
         <f t="shared" ref="U33:U48" si="5">U15</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="V33" s="11">
+      <c r="V33" s="10">
         <v>0.6</v>
       </c>
-      <c r="W33" s="11">
+      <c r="W33" s="10">
         <v>0.02</v>
       </c>
-      <c r="X33" s="11">
+      <c r="X33" s="10">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="Y33" s="11">
+      <c r="Y33" s="10">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="Z33" s="8">
@@ -8247,7 +8245,7 @@
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="9" t="s">
         <v>209</v>
       </c>
       <c r="B34" s="8">
@@ -8289,19 +8287,19 @@
       </c>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
-      <c r="P34" s="11">
+      <c r="P34" s="10">
         <f t="shared" si="2"/>
         <v>7.2295901639344251</v>
       </c>
-      <c r="Q34" s="11">
+      <c r="Q34" s="10">
         <f t="shared" si="2"/>
         <v>1.7617213114754098</v>
       </c>
-      <c r="R34" s="11">
+      <c r="R34" s="10">
         <f t="shared" si="2"/>
         <v>14.449426229508195</v>
       </c>
-      <c r="S34" s="11">
+      <c r="S34" s="10">
         <f t="shared" si="2"/>
         <v>11.497213114754096</v>
       </c>
@@ -8316,7 +8314,7 @@
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="9" t="s">
         <v>210</v>
       </c>
       <c r="B35" s="8">
@@ -8358,19 +8356,19 @@
       </c>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
-      <c r="P35" s="11">
+      <c r="P35" s="10">
         <f t="shared" si="2"/>
         <v>4.5713114754098365</v>
       </c>
-      <c r="Q35" s="11">
+      <c r="Q35" s="10">
         <f t="shared" si="2"/>
         <v>0.85655737704918022</v>
       </c>
-      <c r="R35" s="11">
+      <c r="R35" s="10">
         <f t="shared" si="2"/>
         <v>8.8337704918032784</v>
       </c>
-      <c r="S35" s="11">
+      <c r="S35" s="10">
         <f t="shared" si="2"/>
         <v>7.1161475409836052</v>
       </c>
@@ -8385,7 +8383,7 @@
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="9" t="s">
         <v>211</v>
       </c>
       <c r="B36" s="8">
@@ -8427,19 +8425,19 @@
       </c>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
-      <c r="P36" s="11">
+      <c r="P36" s="10">
         <f t="shared" si="2"/>
         <v>6.6147540983606562E-2</v>
       </c>
-      <c r="Q36" s="11">
+      <c r="Q36" s="10">
         <f t="shared" si="2"/>
         <v>0.24795081967213117</v>
       </c>
-      <c r="R36" s="11">
+      <c r="R36" s="10">
         <f t="shared" si="2"/>
         <v>0.2439344262295082</v>
       </c>
-      <c r="S36" s="11">
+      <c r="S36" s="10">
         <f t="shared" si="2"/>
         <v>0.30836065573770488</v>
       </c>
@@ -8454,7 +8452,7 @@
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="9" t="s">
         <v>212</v>
       </c>
       <c r="B37" s="8">
@@ -8502,19 +8500,19 @@
         <f>H37</f>
         <v>8.4636427076064216</v>
       </c>
-      <c r="P37" s="11">
+      <c r="P37" s="10">
         <f t="shared" si="2"/>
         <v>4.3852459016393446E-2</v>
       </c>
-      <c r="Q37" s="11">
+      <c r="Q37" s="10">
         <f t="shared" si="2"/>
         <v>4.0163934426229514E-3</v>
       </c>
-      <c r="R37" s="11">
+      <c r="R37" s="10">
         <f t="shared" si="2"/>
         <v>4.5737704918032793E-2</v>
       </c>
-      <c r="S37" s="11">
+      <c r="S37" s="10">
         <f t="shared" si="2"/>
         <v>0.11819672131147541</v>
       </c>
@@ -8529,7 +8527,7 @@
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="9" t="s">
         <v>213</v>
       </c>
       <c r="B38" s="8">
@@ -8577,19 +8575,19 @@
         <f>H38</f>
         <v>0.18785764131193303</v>
       </c>
-      <c r="P38" s="11">
+      <c r="P38" s="10">
         <f t="shared" si="2"/>
         <v>6.6885245901639342E-2</v>
       </c>
-      <c r="Q38" s="11">
+      <c r="Q38" s="10">
         <f t="shared" si="2"/>
         <v>0.18663934426229509</v>
       </c>
-      <c r="R38" s="11">
+      <c r="R38" s="10">
         <f t="shared" si="2"/>
         <v>0.15196721311475411</v>
       </c>
-      <c r="S38" s="11">
+      <c r="S38" s="10">
         <f t="shared" si="2"/>
         <v>9.2622950819672117E-2</v>
       </c>
@@ -8604,7 +8602,7 @@
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="9" t="s">
         <v>214</v>
       </c>
       <c r="B39" s="8">
@@ -8649,19 +8647,19 @@
         <f>H39</f>
         <v>0</v>
       </c>
-      <c r="P39" s="11">
+      <c r="P39" s="10">
         <f t="shared" si="2"/>
         <v>0.64057377049180331</v>
       </c>
-      <c r="Q39" s="11">
+      <c r="Q39" s="10">
         <f t="shared" si="2"/>
         <v>0.99868852459016388</v>
       </c>
-      <c r="R39" s="11">
+      <c r="R39" s="10">
         <f t="shared" si="2"/>
         <v>0.74262295081967222</v>
       </c>
-      <c r="S39" s="11">
+      <c r="S39" s="10">
         <f t="shared" si="2"/>
         <v>0.1781967213114754</v>
       </c>
@@ -8676,7 +8674,7 @@
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="9" t="s">
         <v>215</v>
       </c>
       <c r="B40" s="8">
@@ -8724,19 +8722,19 @@
         <f>H40</f>
         <v>0.55987438939288203</v>
       </c>
-      <c r="P40" s="11">
+      <c r="P40" s="10">
         <f t="shared" si="2"/>
         <v>7.1967213114754097E-2</v>
       </c>
-      <c r="Q40" s="11">
+      <c r="Q40" s="10">
         <f t="shared" si="2"/>
         <v>3.2950819672131149E-2</v>
       </c>
-      <c r="R40" s="11">
+      <c r="R40" s="10">
         <f t="shared" si="2"/>
         <v>0.1119672131147541</v>
       </c>
-      <c r="S40" s="11">
+      <c r="S40" s="10">
         <f t="shared" si="2"/>
         <v>3.6393442622950821E-2</v>
       </c>
@@ -8751,7 +8749,7 @@
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="9" t="s">
         <v>216</v>
       </c>
       <c r="B41" s="8">
@@ -8760,7 +8758,7 @@
       <c r="C41" s="8">
         <v>5.9469026548672572E-3</v>
       </c>
-      <c r="D41" s="17"/>
+      <c r="D41" s="16"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
@@ -8775,19 +8773,19 @@
       </c>
       <c r="N41" s="8"/>
       <c r="O41" s="8"/>
-      <c r="P41" s="11">
+      <c r="P41" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q41" s="11">
+      <c r="Q41" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R41" s="11">
+      <c r="R41" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S41" s="11">
+      <c r="S41" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8799,7 +8797,7 @@
       <c r="Z41" s="8"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="9" t="s">
         <v>217</v>
       </c>
       <c r="B42" s="8">
@@ -8808,7 +8806,7 @@
       <c r="C42" s="8">
         <v>1.7964601769911506E-3</v>
       </c>
-      <c r="D42" s="17"/>
+      <c r="D42" s="16"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
@@ -8823,19 +8821,19 @@
       </c>
       <c r="N42" s="8"/>
       <c r="O42" s="8"/>
-      <c r="P42" s="11">
+      <c r="P42" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="11">
+      <c r="Q42" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R42" s="11">
+      <c r="R42" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S42" s="11">
+      <c r="S42" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8847,7 +8845,7 @@
       <c r="Z42" s="8"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
         <v>218</v>
       </c>
       <c r="B43" s="8">
@@ -8856,7 +8854,7 @@
       <c r="C43" s="8">
         <v>2.168141592920354E-3</v>
       </c>
-      <c r="D43" s="17"/>
+      <c r="D43" s="16"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
@@ -8871,19 +8869,19 @@
       </c>
       <c r="N43" s="8"/>
       <c r="O43" s="8"/>
-      <c r="P43" s="11">
+      <c r="P43" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q43" s="11">
+      <c r="Q43" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R43" s="11">
+      <c r="R43" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S43" s="11">
+      <c r="S43" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8895,7 +8893,7 @@
       <c r="Z43" s="8"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="9" t="s">
         <v>219</v>
       </c>
       <c r="B44" s="8">
@@ -8904,7 +8902,7 @@
       <c r="C44" s="8">
         <v>3.3097345132743362E-3</v>
       </c>
-      <c r="D44" s="17"/>
+      <c r="D44" s="16"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
@@ -8919,19 +8917,19 @@
       </c>
       <c r="N44" s="8"/>
       <c r="O44" s="8"/>
-      <c r="P44" s="11">
+      <c r="P44" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q44" s="11">
+      <c r="Q44" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R44" s="11">
+      <c r="R44" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S44" s="11">
+      <c r="S44" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8943,7 +8941,7 @@
       <c r="Z44" s="8"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="9" t="s">
         <v>220</v>
       </c>
       <c r="B45" s="8">
@@ -8952,7 +8950,7 @@
       <c r="C45" s="8">
         <v>4.6017699115044256E-4</v>
       </c>
-      <c r="D45" s="17"/>
+      <c r="D45" s="16"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -8967,19 +8965,19 @@
       </c>
       <c r="N45" s="8"/>
       <c r="O45" s="8"/>
-      <c r="P45" s="11">
+      <c r="P45" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q45" s="11">
+      <c r="Q45" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R45" s="11">
+      <c r="R45" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S45" s="11">
+      <c r="S45" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8991,7 +8989,7 @@
       <c r="Z45" s="8"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="9" t="s">
         <v>221</v>
       </c>
       <c r="B46" s="8">
@@ -9000,7 +8998,7 @@
       <c r="C46" s="8">
         <v>2.4424778761061947E-2</v>
       </c>
-      <c r="D46" s="17"/>
+      <c r="D46" s="16"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -9039,7 +9037,7 @@
       <c r="Z46" s="8"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="9" t="s">
         <v>222</v>
       </c>
       <c r="B47" s="8">
@@ -9048,7 +9046,7 @@
       <c r="C47" s="8">
         <v>1.2743362831858409E-3</v>
       </c>
-      <c r="D47" s="17"/>
+      <c r="D47" s="16"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
@@ -9063,19 +9061,19 @@
       </c>
       <c r="N47" s="8"/>
       <c r="O47" s="8"/>
-      <c r="P47" s="11">
+      <c r="P47" s="10">
         <f>P29</f>
         <v>0</v>
       </c>
-      <c r="Q47" s="11">
+      <c r="Q47" s="10">
         <f t="shared" ref="Q47:S47" si="17">Q29</f>
         <v>0</v>
       </c>
-      <c r="R47" s="11">
+      <c r="R47" s="10">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="S47" s="11">
+      <c r="S47" s="10">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -9086,8 +9084,8 @@
       </c>
       <c r="Z47" s="8"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A48" s="10" t="s">
+    <row r="48" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="9" t="s">
         <v>223</v>
       </c>
       <c r="B48" s="8">
@@ -9130,19 +9128,19 @@
       </c>
       <c r="N48" s="8"/>
       <c r="O48" s="8"/>
-      <c r="P48" s="11">
+      <c r="P48" s="10">
         <f t="shared" ref="P48:S48" si="18">P30</f>
         <v>87.284180327868853</v>
       </c>
-      <c r="Q48" s="11">
+      <c r="Q48" s="10">
         <f t="shared" si="18"/>
         <v>78.597295081967218</v>
       </c>
-      <c r="R48" s="11">
+      <c r="R48" s="10">
         <f t="shared" si="18"/>
         <v>93.389590163934429</v>
       </c>
-      <c r="S48" s="11">
+      <c r="S48" s="10">
         <f t="shared" si="18"/>
         <v>74.067578772802662</v>
       </c>
@@ -9156,801 +9154,793 @@
         <v>93.389590163934429</v>
       </c>
     </row>
-    <row r="49" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="18" t="s">
+    <row r="49" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="19">
+      <c r="B49" s="25">
         <v>13335654.81024</v>
       </c>
-      <c r="C49" s="19">
+      <c r="C49" s="25">
         <v>2030000</v>
       </c>
-      <c r="D49" s="19">
+      <c r="D49" s="25">
         <v>202500000</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E49" s="25">
         <v>12605000</v>
       </c>
-      <c r="F49" s="19">
+      <c r="F49" s="25">
         <v>40000000</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G49" s="25">
         <v>5000000</v>
       </c>
-      <c r="H49" s="19">
+      <c r="H49" s="25">
         <v>20000000</v>
       </c>
-      <c r="L49" s="19">
+      <c r="L49" s="25">
         <v>25000000</v>
       </c>
-      <c r="M49" s="19">
+      <c r="M49" s="25">
         <v>24000000</v>
       </c>
-      <c r="N49" s="19">
+      <c r="N49" s="25">
         <v>45000000</v>
       </c>
-      <c r="O49" s="19">
+      <c r="O49" s="25">
         <v>24000000</v>
       </c>
-      <c r="T49" s="19">
+      <c r="T49" s="25">
         <v>15200000</v>
       </c>
-      <c r="U49" s="19">
+      <c r="U49" s="25">
         <v>40000000</v>
       </c>
-      <c r="V49" s="19">
+      <c r="V49" s="25">
         <v>10000000</v>
       </c>
-      <c r="W49" s="19">
+      <c r="W49" s="25">
         <v>25000000</v>
       </c>
-      <c r="X49" s="19">
+      <c r="X49" s="25">
         <v>10000000</v>
       </c>
-      <c r="Z49" s="19">
+      <c r="Z49" s="25">
         <v>20000000</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A50" s="10" t="s">
+    <row r="50" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B50" s="11">
-        <f>365*90%</f>
+      <c r="B50" s="26">
         <v>328.5</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="26">
         <v>328.5</v>
       </c>
-      <c r="D50" s="11">
+      <c r="D50" s="26">
         <v>365</v>
       </c>
-      <c r="E50" s="12">
+      <c r="E50" s="26">
         <v>365</v>
       </c>
-      <c r="F50" s="11">
+      <c r="F50" s="26">
         <v>292</v>
       </c>
-      <c r="G50" s="12">
+      <c r="G50" s="26">
         <v>360</v>
       </c>
-      <c r="H50" s="11">
+      <c r="H50" s="26">
         <v>328.5</v>
       </c>
-      <c r="L50" s="11">
-        <f>0.8*365</f>
+      <c r="L50" s="26">
         <v>292</v>
       </c>
-      <c r="M50" s="11">
-        <f>365 *0.9</f>
+      <c r="M50" s="26">
         <v>328.5</v>
       </c>
-      <c r="N50" s="11">
+      <c r="N50" s="26">
         <v>333</v>
       </c>
-      <c r="O50" s="11">
-        <f>0.9*365</f>
+      <c r="O50" s="26">
         <v>328.5</v>
       </c>
-      <c r="V50" s="11">
+      <c r="V50" s="26">
         <v>365</v>
       </c>
-      <c r="X50" s="11">
+      <c r="X50" s="26">
         <v>300</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A51" s="10" t="s">
+    <row r="51" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="26">
         <v>30</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="26">
         <v>30</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D51" s="26">
         <v>40</v>
       </c>
-      <c r="E51" s="12">
+      <c r="E51" s="26">
         <v>40</v>
       </c>
-      <c r="F51" s="11">
+      <c r="F51" s="26">
         <v>40</v>
       </c>
-      <c r="G51" s="12">
+      <c r="G51" s="26">
         <v>30</v>
       </c>
-      <c r="H51" s="11">
+      <c r="H51" s="26">
         <v>50</v>
       </c>
-      <c r="M51" s="11">
+      <c r="M51" s="26">
         <v>40</v>
       </c>
-      <c r="N51" s="11">
+      <c r="N51" s="26">
         <v>40</v>
       </c>
-      <c r="O51" s="11">
+      <c r="O51" s="26">
         <v>40</v>
       </c>
-      <c r="T51" s="11">
+      <c r="T51" s="26">
         <v>20</v>
       </c>
-      <c r="V51" s="11">
+      <c r="V51" s="26">
         <v>30</v>
       </c>
-      <c r="W51" s="11">
+      <c r="W51" s="26">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A52" s="10" t="s">
+    <row r="52" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52" s="26">
         <v>437</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="26">
         <v>80</v>
       </c>
-      <c r="D52" s="20">
-        <f>477.4* (D49/70000000)</f>
+      <c r="D52" s="27">
         <v>1381.05</v>
       </c>
-      <c r="E52" s="11">
+      <c r="E52" s="26">
         <v>180</v>
       </c>
-      <c r="F52" s="11">
+      <c r="F52" s="26">
         <v>903</v>
       </c>
-      <c r="G52" s="12">
+      <c r="G52" s="26">
         <v>100</v>
       </c>
-      <c r="H52" s="11">
+      <c r="H52" s="26">
         <v>260</v>
       </c>
-      <c r="L52" s="11">
+      <c r="L52" s="26">
         <v>776</v>
       </c>
-      <c r="M52" s="11">
+      <c r="M52" s="26">
         <v>491.7</v>
       </c>
-      <c r="N52" s="11">
+      <c r="N52" s="26">
         <v>100</v>
       </c>
-      <c r="O52" s="11">
+      <c r="O52" s="26">
         <v>600</v>
       </c>
-      <c r="T52" s="11">
+      <c r="T52" s="26">
         <v>150</v>
       </c>
-      <c r="V52" s="11">
+      <c r="V52" s="26">
         <v>116.67</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A53" s="10" t="s">
+    <row r="53" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B53" s="11">
-        <v>0</v>
-      </c>
-      <c r="C53" s="11">
-        <v>0</v>
-      </c>
-      <c r="D53" s="11">
+      <c r="B53" s="26">
+        <v>0</v>
+      </c>
+      <c r="C53" s="26">
+        <v>0</v>
+      </c>
+      <c r="D53" s="26">
         <v>1</v>
       </c>
-      <c r="E53" s="11">
+      <c r="E53" s="26">
         <v>1</v>
       </c>
-      <c r="F53" s="11">
-        <v>0</v>
-      </c>
-      <c r="G53" s="12">
+      <c r="F53" s="26">
+        <v>0</v>
+      </c>
+      <c r="G53" s="26">
         <v>1</v>
       </c>
-      <c r="H53" s="11">
+      <c r="H53" s="26">
         <v>1</v>
       </c>
-      <c r="J53" s="11">
-        <v>0</v>
-      </c>
-      <c r="L53" s="11">
-        <v>0</v>
-      </c>
-      <c r="M53" s="11">
+      <c r="J53" s="26">
+        <v>0</v>
+      </c>
+      <c r="L53" s="26">
+        <v>0</v>
+      </c>
+      <c r="M53" s="26">
         <v>1</v>
       </c>
-      <c r="N53" s="11">
-        <v>0</v>
-      </c>
-      <c r="O53" s="11">
+      <c r="N53" s="26">
+        <v>0</v>
+      </c>
+      <c r="O53" s="26">
         <v>1</v>
       </c>
-      <c r="T53" s="11">
+      <c r="T53" s="26">
         <v>1</v>
       </c>
-      <c r="V53" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A54" s="10" t="s">
+      <c r="V53" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D54" s="19">
-        <f>31* (D49/70000000)</f>
+      <c r="D54" s="28">
         <v>89.678571428571431</v>
       </c>
-      <c r="E54" s="11">
+      <c r="E54" s="26">
         <v>22</v>
       </c>
-      <c r="F54" s="11">
+      <c r="F54" s="26">
         <v>105</v>
       </c>
-      <c r="G54" s="11">
+      <c r="G54" s="26">
         <v>4.2699999999999996</v>
       </c>
-      <c r="H54" s="11">
+      <c r="H54" s="26">
         <v>14</v>
       </c>
-      <c r="M54" s="11">
+      <c r="M54" s="26">
         <v>98.7</v>
       </c>
-      <c r="O54" s="11">
+      <c r="O54" s="26">
         <v>35</v>
       </c>
-      <c r="T54" s="11">
+      <c r="T54" s="26">
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A55" s="10" t="s">
+    <row r="55" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="11">
+      <c r="B55" s="26">
         <v>0.5</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="26">
         <v>0.5</v>
       </c>
-      <c r="D55" s="11">
+      <c r="D55" s="26">
         <v>0.35</v>
       </c>
-      <c r="E55" s="11">
+      <c r="E55" s="26">
         <v>0.45</v>
       </c>
-      <c r="F55" s="11">
+      <c r="F55" s="26">
         <v>0.53</v>
       </c>
-      <c r="G55" s="12">
+      <c r="G55" s="26">
         <v>0.46</v>
       </c>
-      <c r="H55" s="11">
+      <c r="H55" s="26">
         <v>0.51</v>
       </c>
-      <c r="I55" s="11">
+      <c r="I55" s="26">
         <v>0.77</v>
       </c>
-      <c r="J55" s="11">
+      <c r="J55" s="26">
         <v>0.77</v>
       </c>
-      <c r="K55" s="11">
+      <c r="K55" s="26">
         <v>0.77</v>
       </c>
-      <c r="L55" s="11">
+      <c r="L55" s="26">
         <v>0.77</v>
       </c>
-      <c r="M55" s="11">
+      <c r="M55" s="26">
         <v>0.77</v>
       </c>
-      <c r="N55" s="11">
+      <c r="N55" s="26">
         <v>0.5</v>
       </c>
-      <c r="O55" s="11">
+      <c r="O55" s="26">
         <v>0.61</v>
       </c>
-      <c r="P55" s="11">
+      <c r="P55" s="26">
         <v>0.77</v>
       </c>
-      <c r="Q55" s="11">
+      <c r="Q55" s="26">
         <v>0.77</v>
       </c>
-      <c r="R55" s="11">
+      <c r="R55" s="26">
         <v>0.77</v>
       </c>
-      <c r="S55" s="11">
+      <c r="S55" s="26">
         <v>0.77</v>
       </c>
-      <c r="T55" s="11">
+      <c r="T55" s="26">
         <v>0.57999999999999996</v>
       </c>
-      <c r="U55" s="11">
+      <c r="U55" s="26">
         <v>0.77</v>
       </c>
-      <c r="V55" s="11">
+      <c r="V55" s="26">
         <v>0.51</v>
       </c>
-      <c r="W55" s="11">
+      <c r="W55" s="26">
         <v>0.77</v>
       </c>
-      <c r="X55" s="11">
+      <c r="X55" s="26">
         <v>0.77</v>
       </c>
-      <c r="Y55" s="11">
+      <c r="Y55" s="26">
         <v>0.77</v>
       </c>
-      <c r="Z55" s="11">
+      <c r="Z55" s="26">
         <v>0.77</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A56" s="10" t="s">
+    <row r="56" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F56" s="11">
+      <c r="F56" s="26">
         <v>40</v>
       </c>
-      <c r="N56" s="11">
+      <c r="N56" s="26">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A57" s="10" t="s">
+    <row r="57" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="11">
+      <c r="B57" s="26">
         <v>1500</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="26">
         <v>3600</v>
       </c>
-      <c r="D57" s="11">
+      <c r="D57" s="26">
         <v>50</v>
       </c>
-      <c r="E57" s="11">
+      <c r="E57" s="26">
         <v>50</v>
       </c>
-      <c r="F57" s="11">
+      <c r="F57" s="26">
         <v>10</v>
       </c>
-      <c r="G57" s="12">
+      <c r="G57" s="26">
         <v>50</v>
       </c>
-      <c r="H57" s="11">
+      <c r="H57" s="26">
         <v>400</v>
       </c>
-      <c r="L57" s="11">
+      <c r="L57" s="26">
         <v>380</v>
       </c>
-      <c r="M57" s="11">
+      <c r="M57" s="26">
         <v>55</v>
       </c>
-      <c r="N57" s="11">
+      <c r="N57" s="26">
         <v>280</v>
       </c>
-      <c r="O57" s="11">
+      <c r="O57" s="26">
         <v>540</v>
       </c>
-      <c r="T57" s="11">
+      <c r="T57" s="26">
         <v>130</v>
       </c>
-      <c r="V57" s="11">
+      <c r="V57" s="26">
         <v>200</v>
       </c>
-      <c r="W57" s="11">
+      <c r="W57" s="26">
         <v>400</v>
       </c>
-      <c r="X57" s="11">
+      <c r="X57" s="26">
         <v>20</v>
       </c>
-      <c r="Y57" s="11">
+      <c r="Y57" s="26">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A58" s="10" t="s">
+    <row r="58" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B58" s="11">
-        <v>0</v>
-      </c>
-      <c r="C58" s="11">
-        <v>0</v>
-      </c>
-      <c r="D58" s="11">
+      <c r="B58" s="26">
+        <v>0</v>
+      </c>
+      <c r="C58" s="26">
+        <v>0</v>
+      </c>
+      <c r="D58" s="26">
         <v>10</v>
       </c>
-      <c r="O58" s="11">
+      <c r="O58" s="26">
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A59" s="10" t="s">
+    <row r="59" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B59" s="11">
-        <v>0</v>
-      </c>
-      <c r="C59" s="11">
-        <v>0</v>
-      </c>
-      <c r="D59" s="11">
+      <c r="B59" s="26">
+        <v>0</v>
+      </c>
+      <c r="C59" s="26">
+        <v>0</v>
+      </c>
+      <c r="D59" s="26">
         <v>240</v>
       </c>
-      <c r="E59" s="11">
-        <v>0</v>
-      </c>
-      <c r="F59" s="11">
-        <v>0</v>
-      </c>
-      <c r="G59" s="11">
-        <v>0</v>
-      </c>
-      <c r="H59" s="11">
+      <c r="E59" s="26">
+        <v>0</v>
+      </c>
+      <c r="F59" s="26">
+        <v>0</v>
+      </c>
+      <c r="G59" s="26">
+        <v>0</v>
+      </c>
+      <c r="H59" s="26">
         <v>160</v>
       </c>
-      <c r="L59" s="11">
-        <v>0</v>
-      </c>
-      <c r="V59" s="11">
-        <v>0</v>
-      </c>
-      <c r="X59" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y59" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A60" s="10" t="s">
+      <c r="L59" s="26">
+        <v>0</v>
+      </c>
+      <c r="V59" s="26">
+        <v>0</v>
+      </c>
+      <c r="X59" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y59" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B60" s="11">
-        <v>0</v>
-      </c>
-      <c r="C60" s="11">
-        <v>0</v>
-      </c>
-      <c r="D60" s="11">
-        <v>0</v>
-      </c>
-      <c r="E60" s="11">
+      <c r="B60" s="26">
+        <v>0</v>
+      </c>
+      <c r="C60" s="26">
+        <v>0</v>
+      </c>
+      <c r="D60" s="26">
+        <v>0</v>
+      </c>
+      <c r="E60" s="26">
         <v>1</v>
       </c>
-      <c r="F60" s="11">
+      <c r="F60" s="26">
         <v>1</v>
       </c>
-      <c r="G60" s="11">
+      <c r="G60" s="26">
         <v>1</v>
       </c>
-      <c r="H60" s="11">
-        <v>0</v>
-      </c>
-      <c r="I60" s="11">
-        <v>0</v>
-      </c>
-      <c r="J60" s="11">
-        <v>0</v>
-      </c>
-      <c r="K60" s="11">
-        <v>0</v>
-      </c>
-      <c r="L60" s="11">
-        <v>0</v>
-      </c>
-      <c r="M60" s="11">
-        <v>0</v>
-      </c>
-      <c r="N60" s="11">
+      <c r="H60" s="26">
+        <v>0</v>
+      </c>
+      <c r="I60" s="26">
+        <v>0</v>
+      </c>
+      <c r="J60" s="26">
+        <v>0</v>
+      </c>
+      <c r="K60" s="26">
+        <v>0</v>
+      </c>
+      <c r="L60" s="26">
+        <v>0</v>
+      </c>
+      <c r="M60" s="26">
+        <v>0</v>
+      </c>
+      <c r="N60" s="26">
         <v>1</v>
       </c>
-      <c r="O60" s="11">
+      <c r="O60" s="26">
         <v>1</v>
       </c>
-      <c r="P60" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q60" s="11">
-        <v>0</v>
-      </c>
-      <c r="R60" s="11">
-        <v>0</v>
-      </c>
-      <c r="S60" s="11">
-        <v>0</v>
-      </c>
-      <c r="T60" s="11">
-        <v>0</v>
-      </c>
-      <c r="U60" s="11">
-        <f>(Sheet2!Q47/(1000*Sheet1!$U$13))*100</f>
-        <v>0</v>
-      </c>
-      <c r="V60" s="11">
+      <c r="P60" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="26">
+        <v>0</v>
+      </c>
+      <c r="R60" s="26">
+        <v>0</v>
+      </c>
+      <c r="S60" s="26">
+        <v>0</v>
+      </c>
+      <c r="T60" s="26">
+        <v>0</v>
+      </c>
+      <c r="U60" s="26">
+        <v>0</v>
+      </c>
+      <c r="V60" s="26">
         <v>1</v>
       </c>
-      <c r="W60" s="11">
-        <v>0</v>
-      </c>
-      <c r="X60" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A61" s="10" t="s">
+      <c r="W60" s="26">
+        <v>0</v>
+      </c>
+      <c r="X60" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="26">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B61" s="11">
-        <v>0</v>
-      </c>
-      <c r="C61" s="11">
-        <v>0</v>
-      </c>
-      <c r="D61" s="11">
-        <v>0</v>
-      </c>
-      <c r="E61" s="11">
-        <v>0</v>
-      </c>
-      <c r="F61" s="11">
+      <c r="B61" s="26">
+        <v>0</v>
+      </c>
+      <c r="C61" s="26">
+        <v>0</v>
+      </c>
+      <c r="D61" s="26">
+        <v>0</v>
+      </c>
+      <c r="E61" s="26">
+        <v>0</v>
+      </c>
+      <c r="F61" s="26">
         <v>1</v>
       </c>
-      <c r="G61" s="11">
-        <v>0</v>
-      </c>
-      <c r="H61" s="11">
+      <c r="G61" s="26">
+        <v>0</v>
+      </c>
+      <c r="H61" s="26">
         <v>1</v>
       </c>
-      <c r="I61" s="11">
-        <v>0</v>
-      </c>
-      <c r="J61" s="11">
-        <v>0</v>
-      </c>
-      <c r="K61" s="11">
-        <v>0</v>
-      </c>
-      <c r="L61" s="11">
-        <v>0</v>
-      </c>
-      <c r="M61" s="11">
-        <v>0</v>
-      </c>
-      <c r="N61" s="11">
+      <c r="I61" s="26">
+        <v>0</v>
+      </c>
+      <c r="J61" s="26">
+        <v>0</v>
+      </c>
+      <c r="K61" s="26">
+        <v>0</v>
+      </c>
+      <c r="L61" s="26">
+        <v>0</v>
+      </c>
+      <c r="M61" s="26">
+        <v>0</v>
+      </c>
+      <c r="N61" s="26">
         <v>1</v>
       </c>
-      <c r="O61" s="11">
-        <v>0</v>
-      </c>
-      <c r="P61" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="11">
-        <v>0</v>
-      </c>
-      <c r="R61" s="11">
-        <v>0</v>
-      </c>
-      <c r="S61" s="11">
-        <v>0</v>
-      </c>
-      <c r="T61" s="11">
-        <v>0</v>
-      </c>
-      <c r="U61" s="11">
-        <v>0</v>
-      </c>
-      <c r="V61" s="11">
-        <v>0</v>
-      </c>
-      <c r="W61" s="11">
-        <v>0</v>
-      </c>
-      <c r="X61" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y61" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A62" s="10" t="s">
+      <c r="O61" s="26">
+        <v>0</v>
+      </c>
+      <c r="P61" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="26">
+        <v>0</v>
+      </c>
+      <c r="R61" s="26">
+        <v>0</v>
+      </c>
+      <c r="S61" s="26">
+        <v>0</v>
+      </c>
+      <c r="T61" s="26">
+        <v>0</v>
+      </c>
+      <c r="U61" s="26">
+        <v>0</v>
+      </c>
+      <c r="V61" s="26">
+        <v>0</v>
+      </c>
+      <c r="W61" s="26">
+        <v>0</v>
+      </c>
+      <c r="X61" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y61" s="26">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="F62" s="11">
+      <c r="F62" s="26">
         <v>4</v>
       </c>
-      <c r="H62" s="11">
+      <c r="H62" s="26">
         <v>3.2</v>
       </c>
-      <c r="N62" s="11">
+      <c r="N62" s="26">
         <v>1.7</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A63" s="10" t="s">
+    <row r="63" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B63" s="11">
-        <v>0</v>
-      </c>
-      <c r="C63" s="11">
-        <v>0</v>
-      </c>
-      <c r="D63" s="11">
+      <c r="B63" s="26">
+        <v>0</v>
+      </c>
+      <c r="C63" s="26">
+        <v>0</v>
+      </c>
+      <c r="D63" s="26">
         <v>1</v>
       </c>
-      <c r="E63" s="11">
-        <v>0</v>
-      </c>
-      <c r="F63" s="11">
-        <v>0</v>
-      </c>
-      <c r="G63" s="11">
-        <v>0</v>
-      </c>
-      <c r="H63" s="11">
-        <v>0</v>
-      </c>
-      <c r="T63" s="11">
-        <v>0</v>
-      </c>
-      <c r="V63" s="11">
-        <v>0</v>
-      </c>
-      <c r="X63" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y63" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A64" s="10" t="s">
+      <c r="E63" s="26">
+        <v>0</v>
+      </c>
+      <c r="F63" s="26">
+        <v>0</v>
+      </c>
+      <c r="G63" s="26">
+        <v>0</v>
+      </c>
+      <c r="H63" s="26">
+        <v>0</v>
+      </c>
+      <c r="T63" s="26">
+        <v>0</v>
+      </c>
+      <c r="V63" s="26">
+        <v>0</v>
+      </c>
+      <c r="X63" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y63" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D64" s="21">
-        <f>1557778* (D49/70000000)</f>
+      <c r="D64" s="27">
         <v>4506429.2142857146</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A65" s="10" t="s">
+    <row r="65" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B65" s="11">
-        <v>0</v>
-      </c>
-      <c r="C65" s="11">
-        <v>0</v>
-      </c>
-      <c r="D65" s="11">
+      <c r="B65" s="26">
+        <v>0</v>
+      </c>
+      <c r="C65" s="26">
+        <v>0</v>
+      </c>
+      <c r="D65" s="26">
         <v>1</v>
       </c>
-      <c r="E65" s="11">
+      <c r="E65" s="26">
         <v>1</v>
       </c>
-      <c r="F65" s="11">
+      <c r="F65" s="26">
         <v>1</v>
       </c>
-      <c r="G65" s="11">
+      <c r="G65" s="26">
         <v>1</v>
       </c>
-      <c r="H65" s="11">
+      <c r="H65" s="26">
         <v>1</v>
       </c>
-      <c r="I65" s="11">
-        <v>0</v>
-      </c>
-      <c r="J65" s="11">
-        <v>0</v>
-      </c>
-      <c r="K65" s="11">
-        <v>0</v>
-      </c>
-      <c r="L65" s="11">
-        <v>0</v>
-      </c>
-      <c r="M65" s="11">
-        <v>0</v>
-      </c>
-      <c r="N65" s="11">
-        <v>0</v>
-      </c>
-      <c r="O65" s="11">
-        <v>0</v>
-      </c>
-      <c r="P65" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q65" s="11">
-        <v>0</v>
-      </c>
-      <c r="R65" s="11">
-        <v>0</v>
-      </c>
-      <c r="S65" s="11">
-        <v>0</v>
-      </c>
-      <c r="T65" s="11">
+      <c r="I65" s="26">
+        <v>0</v>
+      </c>
+      <c r="J65" s="26">
+        <v>0</v>
+      </c>
+      <c r="K65" s="26">
+        <v>0</v>
+      </c>
+      <c r="L65" s="26">
+        <v>0</v>
+      </c>
+      <c r="M65" s="26">
+        <v>0</v>
+      </c>
+      <c r="N65" s="26">
+        <v>0</v>
+      </c>
+      <c r="O65" s="26">
+        <v>0</v>
+      </c>
+      <c r="P65" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="26">
+        <v>0</v>
+      </c>
+      <c r="R65" s="26">
+        <v>0</v>
+      </c>
+      <c r="S65" s="26">
+        <v>0</v>
+      </c>
+      <c r="T65" s="26">
         <v>1</v>
       </c>
-      <c r="U65" s="11">
-        <v>0</v>
-      </c>
-      <c r="V65" s="11">
+      <c r="U65" s="26">
+        <v>0</v>
+      </c>
+      <c r="V65" s="26">
         <v>1</v>
       </c>
-      <c r="W65" s="11">
-        <v>0</v>
-      </c>
-      <c r="X65" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y65" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z65" s="11">
+      <c r="W65" s="26">
+        <v>0</v>
+      </c>
+      <c r="X65" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="26">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E66" s="11">
+      <c r="E66" s="10">
         <v>128340</v>
       </c>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A67" s="10" t="s">
+      <c r="A67" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="O67" s="11" t="s">
+      <c r="O67" s="10" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A69" s="22" t="s">
+      <c r="A69" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="E69" s="20"/>
+      <c r="E69" s="17"/>
     </row>
     <row r="70" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="19" t="s">
         <v>129</v>
       </c>
       <c r="B70" s="8" t="s">
@@ -10030,7 +10020,7 @@
       </c>
     </row>
     <row r="71" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="23" t="s">
+      <c r="A71" s="19" t="s">
         <v>130</v>
       </c>
       <c r="B71" s="8" t="s">
@@ -10110,7 +10100,7 @@
       </c>
     </row>
     <row r="72" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="23" t="s">
+      <c r="A72" s="19" t="s">
         <v>131</v>
       </c>
       <c r="B72" s="8" t="s">
@@ -10190,7 +10180,7 @@
       </c>
     </row>
     <row r="73" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="23" t="s">
+      <c r="A73" s="19" t="s">
         <v>132</v>
       </c>
       <c r="B73" s="8" t="s">
@@ -10270,7 +10260,7 @@
       </c>
     </row>
     <row r="74" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="19" t="s">
         <v>133</v>
       </c>
       <c r="B74" s="8" t="s">
@@ -10350,7 +10340,7 @@
       </c>
     </row>
     <row r="75" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="23" t="s">
+      <c r="A75" s="19" t="s">
         <v>134</v>
       </c>
       <c r="B75" s="8" t="s">
@@ -10430,7 +10420,7 @@
       </c>
     </row>
     <row r="76" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="23" t="s">
+      <c r="A76" s="19" t="s">
         <v>135</v>
       </c>
       <c r="B76" s="8" t="s">
@@ -10510,7 +10500,7 @@
       </c>
     </row>
     <row r="77" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="23" t="s">
+      <c r="A77" s="19" t="s">
         <v>136</v>
       </c>
       <c r="B77" s="8" t="s">
@@ -10590,7 +10580,7 @@
       </c>
     </row>
     <row r="78" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="23" t="s">
+      <c r="A78" s="19" t="s">
         <v>137</v>
       </c>
       <c r="B78" s="8" t="s">
@@ -10670,7 +10660,7 @@
       </c>
     </row>
     <row r="79" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="19" t="s">
         <v>138</v>
       </c>
       <c r="B79" s="8" t="s">
@@ -10750,7 +10740,7 @@
       </c>
     </row>
     <row r="80" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="23" t="s">
+      <c r="A80" s="19" t="s">
         <v>139</v>
       </c>
       <c r="B80" s="8" t="s">
@@ -10830,7 +10820,7 @@
       </c>
     </row>
     <row r="81" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="23" t="s">
+      <c r="A81" s="19" t="s">
         <v>140</v>
       </c>
       <c r="B81" s="8" t="s">
@@ -10910,7 +10900,7 @@
       </c>
     </row>
     <row r="82" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="23" t="s">
+      <c r="A82" s="19" t="s">
         <v>141</v>
       </c>
       <c r="B82" s="8" t="s">
@@ -10990,7 +10980,7 @@
       </c>
     </row>
     <row r="83" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="23" t="s">
+      <c r="A83" s="19" t="s">
         <v>142</v>
       </c>
       <c r="B83" s="8" t="s">
@@ -11029,7 +11019,7 @@
       <c r="M83" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="N83" s="11" t="s">
+      <c r="N83" s="10" t="s">
         <v>165</v>
       </c>
       <c r="O83" s="8" t="s">
@@ -11070,7 +11060,7 @@
       </c>
     </row>
     <row r="84" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="23" t="s">
+      <c r="A84" s="19" t="s">
         <v>143</v>
       </c>
       <c r="B84" s="8" t="s">
@@ -11082,7 +11072,7 @@
       <c r="D84" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E84" s="11" t="s">
+      <c r="E84" s="10" t="s">
         <v>165</v>
       </c>
       <c r="F84" s="8" t="s">
@@ -11130,16 +11120,16 @@
       <c r="U84" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="V84" s="11" t="s">
+      <c r="V84" s="10" t="s">
         <v>165</v>
       </c>
       <c r="W84" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="X84" s="11" t="s">
+      <c r="X84" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="Y84" s="11" t="s">
+      <c r="Y84" s="10" t="s">
         <v>165</v>
       </c>
       <c r="Z84" s="8" t="s">
@@ -11147,7 +11137,7 @@
       </c>
     </row>
     <row r="85" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A85" s="23" t="s">
+      <c r="A85" s="19" t="s">
         <v>144</v>
       </c>
       <c r="B85" s="8" t="s">
@@ -11162,103 +11152,103 @@
       <c r="F85" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="G85" s="11" t="s">
+      <c r="G85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="H85" s="11" t="s">
+      <c r="H85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="I85" s="11" t="s">
+      <c r="I85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="J85" s="11" t="s">
+      <c r="J85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="K85" s="11" t="s">
+      <c r="K85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="L85" s="11" t="s">
+      <c r="L85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="M85" s="11" t="s">
+      <c r="M85" s="10" t="s">
         <v>165</v>
       </c>
       <c r="O85" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="P85" s="11" t="s">
+      <c r="P85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="Q85" s="11" t="s">
+      <c r="Q85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="R85" s="11" t="s">
+      <c r="R85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="S85" s="11" t="s">
+      <c r="S85" s="10" t="s">
         <v>165</v>
       </c>
       <c r="T85" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="U85" s="11" t="s">
+      <c r="U85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="W85" s="11" t="s">
+      <c r="W85" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="Z85" s="11" t="s">
+      <c r="Z85" s="10" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A86" s="23" t="s">
+      <c r="A86" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B86" s="11" t="s">
+      <c r="B86" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C86" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="D86" s="11" t="s">
+      <c r="D86" s="10" t="s">
         <v>165</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>164</v>
       </c>
       <c r="H86" s="8"/>
-      <c r="O86" s="11" t="s">
+      <c r="O86" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="T86" s="11" t="s">
+      <c r="T86" s="10" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A87" s="23" t="s">
+      <c r="A87" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="F87" s="11" t="s">
+      <c r="F87" s="10" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A88" s="23" t="s">
+      <c r="A88" s="19" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A89" s="23" t="s">
+      <c r="A89" s="19" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24"/>
-      <c r="H91" s="24"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="20"/>
+      <c r="H91" s="20"/>
       <c r="I91" s="8"/>
       <c r="J91" s="8"/>
       <c r="K91" s="8"/>
@@ -11276,107 +11266,107 @@
       <c r="Y91" s="8"/>
       <c r="Z91" s="8"/>
     </row>
-    <row r="92" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="25" t="s">
-        <v>1783</v>
-      </c>
-      <c r="B92" s="26">
+    <row r="92" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A92" s="21" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B92" s="22">
         <f>SUM(B37:B41,B43,B44,B45)</f>
         <v>2.610849557522124</v>
       </c>
-      <c r="C92" s="26">
+      <c r="C92" s="22">
         <f t="shared" ref="C92:Z92" si="19">SUM(C37:C41,C43,C44,C45)</f>
         <v>0.49976106194690262</v>
       </c>
-      <c r="D92" s="26">
+      <c r="D92" s="22">
         <f>SUM(D37:D41,D43,D44,D45)</f>
         <v>2.6019999999999999</v>
       </c>
-      <c r="E92" s="26">
+      <c r="E92" s="22">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F92" s="26">
+      <c r="F92" s="22">
         <f t="shared" si="19"/>
         <v>3.694</v>
       </c>
-      <c r="G92" s="26">
-        <f t="shared" si="19"/>
+      <c r="G92" s="22">
+        <f>SUM(G37:G41,G43,G44,G45)</f>
         <v>2.9009121061359866</v>
       </c>
-      <c r="H92" s="26">
+      <c r="H92" s="22">
         <f t="shared" si="19"/>
         <v>9.2113747383112354</v>
       </c>
-      <c r="I92" s="26">
+      <c r="I92" s="22">
         <f t="shared" si="19"/>
         <v>1.6392622950819671</v>
       </c>
-      <c r="J92" s="26">
+      <c r="J92" s="22">
         <f t="shared" si="19"/>
         <v>3.1279508196721304</v>
       </c>
-      <c r="K92" s="26">
+      <c r="K92" s="22">
         <f t="shared" si="19"/>
         <v>1.2854918032786884</v>
       </c>
-      <c r="L92" s="26">
+      <c r="L92" s="22">
         <f t="shared" si="19"/>
         <v>0.18733333333333332</v>
       </c>
-      <c r="M92" s="26">
+      <c r="M92" s="22">
         <f t="shared" si="19"/>
         <v>1.0654228855721393</v>
       </c>
-      <c r="N92" s="26">
+      <c r="N92" s="22">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="O92" s="26">
+      <c r="O92" s="22">
         <f t="shared" si="19"/>
         <v>9.2113747383112354</v>
       </c>
-      <c r="P92" s="26">
+      <c r="P92" s="22">
         <f t="shared" si="19"/>
         <v>0.82327868852459019</v>
       </c>
-      <c r="Q92" s="26">
+      <c r="Q92" s="22">
         <f t="shared" si="19"/>
         <v>1.2222950819672129</v>
       </c>
-      <c r="R92" s="26">
+      <c r="R92" s="22">
         <f t="shared" si="19"/>
         <v>1.0522950819672132</v>
       </c>
-      <c r="S92" s="26">
+      <c r="S92" s="22">
         <f t="shared" si="19"/>
         <v>0.42540983606557375</v>
       </c>
-      <c r="T92" s="26">
+      <c r="T92" s="22">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="U92" s="26">
+      <c r="U92" s="22">
         <f>SUM(U37:U41,U43,U44,U45)</f>
         <v>3.5024999999999999</v>
       </c>
-      <c r="V92" s="26">
+      <c r="V92" s="22">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="W92" s="26">
+      <c r="W92" s="22">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="X92" s="26">
+      <c r="X92" s="22">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="Y92" s="26">
+      <c r="Y92" s="22">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="Z92" s="26">
+      <c r="Z92" s="22">
         <f t="shared" si="19"/>
         <v>1.0435245901639345</v>
       </c>
@@ -11422,7 +11412,7 @@
       <c r="Y96" s="8"/>
     </row>
     <row r="101" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E101" s="11">
+      <c r="E101" s="10">
         <f>E66</f>
         <v>128340</v>
       </c>
@@ -11523,7 +11513,7 @@
         <v>119</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.45">
@@ -12453,18 +12443,18 @@
       <c r="B3" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -12584,16 +12574,16 @@
       <c r="L7">
         <v>302</v>
       </c>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="28"/>
-      <c r="V7" s="28"/>
-      <c r="W7" s="28"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="28"/>
-      <c r="Z7" s="28"/>
-      <c r="AA7" s="28"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="24"/>
+      <c r="Z7" s="24"/>
+      <c r="AA7" s="24"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -31397,7 +31387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82FC352-F54F-44E2-863E-F5653510121D}">
   <dimension ref="A1:AD282"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:Q1048576"/>
     </sheetView>
   </sheetViews>
@@ -31493,16 +31483,16 @@
       <c r="I2" s="5">
         <v>530</v>
       </c>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -39511,7 +39501,7 @@
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="B279" s="5">
         <v>47</v>
@@ -39540,7 +39530,7 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A280" t="s">
-        <v>1786</v>
+        <v>1784</v>
       </c>
       <c r="B280" s="5">
         <v>81</v>
@@ -39569,7 +39559,7 @@
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A281" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="B281" s="5">
         <v>235</v>
@@ -39598,7 +39588,7 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A282" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
       <c r="B282" s="5">
         <v>357</v>
@@ -39738,16 +39728,16 @@
       <c r="I2" s="5">
         <v>530</v>
       </c>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -47891,7 +47881,7 @@
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="B279" s="5">
         <v>47</v>
@@ -47920,7 +47910,7 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A280" t="s">
-        <v>1786</v>
+        <v>1784</v>
       </c>
       <c r="B280" s="5">
         <v>81</v>
@@ -47949,7 +47939,7 @@
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A281" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="B281" s="5">
         <v>235</v>
@@ -47978,7 +47968,7 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A282" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
       <c r="B282" s="5">
         <v>357</v>

</xml_diff>

<commit_message>
Update - Structure of the model
</commit_message>
<xml_diff>
--- a/data/new_file_lithiumsites.xlsx
+++ b/data/new_file_lithiumsites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schenker\PycharmProjects\Geothermal_brines\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CBA3C38-E6DF-457B-86A2-8DA864CE2664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B64EE9-3197-4BE1-9E87-EC57463F7872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" tabRatio="704" xr2:uid="{E181E47A-03D8-47CA-9512-5903C9B6271D}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5410" uniqueCount="1793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5476" uniqueCount="1801">
   <si>
     <t>Site name</t>
   </si>
@@ -5419,6 +5419,30 @@
   </si>
   <si>
     <t>Zabuye</t>
+  </si>
+  <si>
+    <t>Zhabuye</t>
+  </si>
+  <si>
+    <t>Zha</t>
+  </si>
+  <si>
+    <t>EaTai</t>
+  </si>
+  <si>
+    <t>Lak</t>
+  </si>
+  <si>
+    <t>Feasibility</t>
+  </si>
+  <si>
+    <t>grinding</t>
+  </si>
+  <si>
+    <t>washing_general</t>
+  </si>
+  <si>
+    <t>electrodialysis</t>
   </si>
 </sst>
 </file>
@@ -5434,7 +5458,7 @@
     <numFmt numFmtId="168" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5478,6 +5502,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -5514,7 +5545,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5576,6 +5607,15 @@
     <xf numFmtId="168" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5687,29 +5727,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B9A88C4-4092-4296-A064-E411E5F9DB7E}" name="Table132" displayName="Table132" ref="A1:Q282" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A1:Q282" xr:uid="{7B9A88C4-4092-4296-A064-E411E5F9DB7E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3CAEBC1-ABD2-4BE2-8216-EF698AD5118D}" name="Table134" displayName="Table134" ref="A1:Q282" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:Q282" xr:uid="{D3CAEBC1-ABD2-4BE2-8216-EF698AD5118D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q278">
     <sortCondition ref="A1:A278"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{9717A187-DC4A-4D4D-B924-EFA8E9056C8F}" name="site_identifier"/>
-    <tableColumn id="2" xr3:uid="{30D97636-695E-4B51-81F4-85E8CD32E753}" name="ini_Li" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{F4AA01F3-56ED-4DB2-B6E2-C8D9F4EA7143}" name="ini_Cl" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{12ADB1B1-F079-49D5-8671-95545F1FBBE4}" name="ini_Na" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{B55ADEDE-1F3E-4815-AD08-FC0E8822BD14}" name="ini_K" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{B94FD87B-7996-40B0-99A6-5546778F3D39}" name="ini_Ca" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{B68E1AE0-DEF9-4666-B308-5CF5DDC1A85F}" name="ini_Mg" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{C2AD89A4-F2F6-42AB-9C4F-63947F91330C}" name="ini_SO4" dataDxfId="10" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{DA1EFC8D-830C-4752-9D44-72FB2BB52671}" name="ini_B" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{E9B7CCC2-1469-4792-847A-CE7AF32BDE06}" name="ini_Si"/>
-    <tableColumn id="11" xr3:uid="{0D927DBA-9975-4C9A-A113-4110038C1258}" name="ini_As"/>
-    <tableColumn id="12" xr3:uid="{3875EF4C-7AAE-43E1-BDD6-64411C09E212}" name="ini_Mn"/>
-    <tableColumn id="13" xr3:uid="{A2AFD5D9-FBDB-4874-9A05-E680B0A21231}" name="ini_Fe"/>
-    <tableColumn id="14" xr3:uid="{61A2F973-6CEA-4407-986C-1636C8919085}" name="ini_Zn"/>
-    <tableColumn id="15" xr3:uid="{B22EF984-257F-4688-AE5A-F99B23BD1D0E}" name="ini_Sr"/>
-    <tableColumn id="16" xr3:uid="{5C87B05A-227C-4903-A0EF-9745A4516473}" name="ini_Ba"/>
-    <tableColumn id="17" xr3:uid="{D3D32F35-A58F-4624-8121-FDB236EE021D}" name="ini_H2O"/>
+    <tableColumn id="1" xr3:uid="{E036A85E-66D6-4CB2-A618-00B93807BC59}" name="site_identifier"/>
+    <tableColumn id="2" xr3:uid="{E2DABD30-711D-4665-9835-3D5DA664204B}" name="ini_Li" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{1DB023E2-8819-45D3-B212-11484276D4E9}" name="ini_Cl" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{BDF79D4D-BFBE-47DB-B35A-9D744208B6CC}" name="ini_Na" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{EB724167-371B-4C4C-BE0E-CE77505EA03B}" name="ini_K" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{9CFBA1A8-597D-4A3B-9F0C-39FC92B76ED6}" name="ini_Ca" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{33911411-BEDA-4FC2-87D3-B90512BA4FFA}" name="ini_Mg" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{20939B81-05DF-4252-BBE0-1844ED14AA18}" name="ini_SO4" dataDxfId="10" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{ABC2B408-A01A-4EE4-886F-B0B744D14FBD}" name="ini_B" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{8A0256CB-C389-4417-B83A-288052EDA773}" name="ini_Si"/>
+    <tableColumn id="11" xr3:uid="{33CD2196-D5CB-4467-8968-F8CA5E4D703C}" name="ini_As"/>
+    <tableColumn id="12" xr3:uid="{8D3BC261-F6FE-435B-953F-350AE1BACD6F}" name="ini_Mn"/>
+    <tableColumn id="13" xr3:uid="{25F787B2-7C9E-4ECA-8F9F-2B517217BF51}" name="ini_Fe"/>
+    <tableColumn id="14" xr3:uid="{79A832F0-C9D4-4CD2-B5D8-F2B96C4684B4}" name="ini_Zn"/>
+    <tableColumn id="15" xr3:uid="{5BCA6119-6E5E-41F6-8602-F293EF6EF51E}" name="ini_Sr"/>
+    <tableColumn id="16" xr3:uid="{53E10AEC-B145-4511-AFD9-B564C5F1A2F6}" name="ini_Ba"/>
+    <tableColumn id="17" xr3:uid="{48B28B10-96BB-465F-9945-3596CE16C995}" name="ini_H2O"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6079,9 +6119,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5319587E-5250-4C3E-BD3D-6C0619F44C22}">
   <dimension ref="A1:AI101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA1" sqref="AA1:AC1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA15" sqref="AA15:AC48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6104,11 +6144,12 @@
     <col min="24" max="24" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.86328125" style="10" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15.265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.73046875" style="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.1328125" style="10"/>
+    <col min="27" max="27" width="16.6640625" style="10" customWidth="1"/>
+    <col min="28" max="28" width="15.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.1328125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -6187,8 +6228,17 @@
       <c r="Z1" s="23" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA1" s="23" t="s">
+        <v>1793</v>
+      </c>
+      <c r="AB1" s="23" t="s">
+        <v>1790</v>
+      </c>
+      <c r="AC1" s="23" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>179</v>
       </c>
@@ -6267,8 +6317,17 @@
       <c r="Z2" s="10" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA2" s="10" t="s">
+        <v>1794</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>1795</v>
+      </c>
+      <c r="AC2" s="10" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
@@ -6347,8 +6406,17 @@
       <c r="Z3" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC3" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>1772</v>
       </c>
@@ -6427,8 +6495,17 @@
       <c r="Z4" s="11" t="s">
         <v>1789</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA4" s="11" t="s">
+        <v>1774</v>
+      </c>
+      <c r="AB4" s="11" t="s">
+        <v>1774</v>
+      </c>
+      <c r="AC4" s="11" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>1767</v>
       </c>
@@ -6507,8 +6584,17 @@
       <c r="Z5" s="11" t="s">
         <v>1769</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA5" s="11" t="s">
+        <v>1770</v>
+      </c>
+      <c r="AB5" s="11" t="s">
+        <v>1769</v>
+      </c>
+      <c r="AC5" s="11" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>41</v>
       </c>
@@ -6588,8 +6674,17 @@
       <c r="Z6" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA6" s="10" t="s">
+        <v>1766</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>1766</v>
+      </c>
+      <c r="AC6" s="10" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>34</v>
       </c>
@@ -6670,8 +6765,17 @@
       <c r="Z7" s="10">
         <v>4060</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA7" s="10">
+        <v>4421</v>
+      </c>
+      <c r="AB7" s="10">
+        <v>2689</v>
+      </c>
+      <c r="AC7" s="10">
+        <v>4506</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>126</v>
       </c>
@@ -6750,8 +6854,17 @@
       <c r="Z8" s="12">
         <v>-66.748329999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA8" s="27">
+        <v>83.947305560000004</v>
+      </c>
+      <c r="AB8" s="27">
+        <v>93.941007459999994</v>
+      </c>
+      <c r="AC8" s="27">
+        <v>84.13549802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>127</v>
       </c>
@@ -6830,8 +6943,17 @@
       <c r="Z9" s="12">
         <v>-25.244720000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA9" s="27">
+        <v>31.35916667</v>
+      </c>
+      <c r="AB9" s="27">
+        <v>37.52255787</v>
+      </c>
+      <c r="AC9" s="27">
+        <v>31.971349329999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>124</v>
       </c>
@@ -6881,7 +7003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>33</v>
       </c>
@@ -6933,8 +7055,14 @@
       <c r="V11" s="10">
         <v>1.425</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA11" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="AB11" s="10">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>35</v>
       </c>
@@ -6971,7 +7099,7 @@
         <v>94.92</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>36</v>
       </c>
@@ -7049,8 +7177,17 @@
       <c r="Z13" s="10">
         <v>1.22</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA13" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="AB13" s="10">
+        <v>1.24</v>
+      </c>
+      <c r="AC13" s="10">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>47</v>
       </c>
@@ -7076,7 +7213,7 @@
       <c r="U14" s="8"/>
       <c r="Z14" s="8"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>193</v>
       </c>
@@ -7169,8 +7306,17 @@
         <f>((Sheet2!Y2/1000)/(Sheet1!$Z$13*1000))*100</f>
         <v>1.9262295081967213E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA15" s="8">
+        <v>7.7857142857142861E-2</v>
+      </c>
+      <c r="AB15" s="8">
+        <v>8.3064516129032262E-2</v>
+      </c>
+      <c r="AC15" s="8">
+        <v>1.6607142857142855E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>194</v>
       </c>
@@ -7245,6 +7391,15 @@
         <f>((Sheet2!Y3/1000)/(Sheet1!$Z$13*1000))*100</f>
         <v>3.1368852459016399</v>
       </c>
+      <c r="AA16" s="8">
+        <v>11.857142857142858</v>
+      </c>
+      <c r="AB16" s="8">
+        <v>14.596774193548386</v>
+      </c>
+      <c r="AC16" s="8">
+        <v>0.69758928571428569</v>
+      </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
@@ -7321,6 +7476,15 @@
         <f>((Sheet2!Y4/1000)/(Sheet1!$Z$13*1000))*100</f>
         <v>1.7651639344262295</v>
       </c>
+      <c r="AA17" s="8">
+        <v>9.7142857142857135</v>
+      </c>
+      <c r="AB17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="8">
+        <v>0.93437499999999996</v>
+      </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
@@ -7403,9 +7567,15 @@
         <f>((Sheet2!Y5/1000)/(Sheet1!$Z$13*1000))*100</f>
         <v>0.64557377049180331</v>
       </c>
-      <c r="AA18" s="15"/>
-      <c r="AB18" s="7"/>
-      <c r="AC18" s="7"/>
+      <c r="AA18" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="8">
+        <v>1.4370967741935483</v>
+      </c>
+      <c r="AC18" s="8">
+        <v>0.16276785714285713</v>
+      </c>
       <c r="AD18" s="7"/>
       <c r="AE18" s="7"/>
       <c r="AF18" s="7"/>
@@ -7491,6 +7661,15 @@
         <f>((Sheet2!Y6/1000)/(Sheet1!$Z$13*1000))*100</f>
         <v>0.11499999999999999</v>
       </c>
+      <c r="AA19" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="8">
+        <v>1.6129032258064516E-2</v>
+      </c>
+      <c r="AC19" s="8">
+        <v>1.0267857142857142E-3</v>
+      </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
@@ -7575,6 +7754,15 @@
       <c r="Z20" s="8">
         <f>((Sheet2!Y7/1000)/(Sheet1!$Z$13*1000))*100</f>
         <v>7.6475409836065572E-2</v>
+      </c>
+      <c r="AA20" s="8">
+        <v>0.37714285714285711</v>
+      </c>
+      <c r="AB20" s="8">
+        <v>2.9225806451612901</v>
+      </c>
+      <c r="AC20" s="8">
+        <v>4.9375000000000002E-2</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.45">
@@ -7655,6 +7843,15 @@
         <f>((Sheet2!Y8/1000)/(Sheet1!$Z$13*1000))*100</f>
         <v>0.78581967213114756</v>
       </c>
+      <c r="AA21" s="8">
+        <v>4.2142857142857144</v>
+      </c>
+      <c r="AB21" s="8">
+        <v>4.6725806451612906</v>
+      </c>
+      <c r="AC21" s="8">
+        <v>1.1236607142857145</v>
+      </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
@@ -7736,6 +7933,15 @@
       <c r="Z22" s="8">
         <f>((Sheet2!Y9/1000)/(Sheet1!$Z$13*1000))*100</f>
         <v>6.6229508196721326E-2</v>
+      </c>
+      <c r="AA22" s="8">
+        <v>0.26071428571428568</v>
+      </c>
+      <c r="AB22" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="8">
+        <v>4.6160714285714291E-2</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.45">
@@ -8047,6 +8253,15 @@
         <f>100-SUM(Z15:Z22)</f>
         <v>93.389590163934429</v>
       </c>
+      <c r="AA30" s="8">
+        <v>73.498571428571424</v>
+      </c>
+      <c r="AB30" s="8">
+        <v>76.271774193548396</v>
+      </c>
+      <c r="AC30" s="8">
+        <v>96.968437499999993</v>
+      </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
@@ -8131,6 +8346,9 @@
       <c r="Z31" s="10">
         <v>1.22</v>
       </c>
+      <c r="AC31" s="10">
+        <v>1.1200000000000001</v>
+      </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
@@ -8154,7 +8372,7 @@
       </c>
       <c r="Z32" s="8"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>208</v>
       </c>
@@ -8245,8 +8463,14 @@
         <f>Z15</f>
         <v>1.9262295081967213E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA33" s="8">
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="AC33" s="10">
+        <v>1.6607142857142855E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>209</v>
       </c>
@@ -8314,8 +8538,11 @@
         <f t="shared" ref="Z34:Z40" si="7">Z16</f>
         <v>3.1368852459016399</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AC34" s="10">
+        <v>0.69758928571428569</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>210</v>
       </c>
@@ -8383,8 +8610,11 @@
         <f t="shared" si="7"/>
         <v>1.7651639344262295</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AC35" s="10">
+        <v>0.93437499999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>211</v>
       </c>
@@ -8452,8 +8682,11 @@
         <f t="shared" si="7"/>
         <v>0.64557377049180331</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AC36" s="10">
+        <v>0.16276785714285713</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>212</v>
       </c>
@@ -8527,8 +8760,11 @@
         <f t="shared" si="7"/>
         <v>0.11499999999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AC37" s="10">
+        <v>1.0267857142857142E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>213</v>
       </c>
@@ -8602,8 +8838,11 @@
         <f t="shared" si="7"/>
         <v>7.6475409836065572E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AC38" s="10">
+        <v>4.9375000000000002E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>214</v>
       </c>
@@ -8674,8 +8913,11 @@
         <f t="shared" si="7"/>
         <v>0.78581967213114756</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AC39" s="10">
+        <v>1.1236607142857145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>215</v>
       </c>
@@ -8749,8 +8991,11 @@
         <f t="shared" si="7"/>
         <v>6.6229508196721326E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AC40" s="10">
+        <v>4.6160714285714291E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>216</v>
       </c>
@@ -8798,7 +9043,7 @@
       </c>
       <c r="Z41" s="8"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>217</v>
       </c>
@@ -8846,7 +9091,7 @@
       </c>
       <c r="Z42" s="8"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
         <v>218</v>
       </c>
@@ -8894,7 +9139,7 @@
       </c>
       <c r="Z43" s="8"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
         <v>219</v>
       </c>
@@ -8942,7 +9187,7 @@
       </c>
       <c r="Z44" s="8"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>220</v>
       </c>
@@ -8990,7 +9235,7 @@
       </c>
       <c r="Z45" s="8"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
         <v>221</v>
       </c>
@@ -9038,7 +9283,7 @@
       </c>
       <c r="Z46" s="8"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A47" s="9" t="s">
         <v>222</v>
       </c>
@@ -9086,7 +9331,7 @@
       </c>
       <c r="Z47" s="8"/>
     </row>
-    <row r="48" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
         <v>223</v>
       </c>
@@ -9155,8 +9400,11 @@
         <f>100-SUM(Z33:Z40)</f>
         <v>93.389590163934429</v>
       </c>
-    </row>
-    <row r="49" spans="1:26" s="24" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AC48" s="10">
+        <v>96.968437499999993</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="24" t="s">
         <v>27</v>
       </c>
@@ -9211,8 +9459,17 @@
       <c r="Z49" s="24">
         <v>20000000</v>
       </c>
-    </row>
-    <row r="50" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA49" s="24">
+        <v>26000000</v>
+      </c>
+      <c r="AB49" s="24">
+        <v>12000000</v>
+      </c>
+      <c r="AC49" s="24">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A50" s="15" t="s">
         <v>28</v>
       </c>
@@ -9256,7 +9513,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="51" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="15" t="s">
         <v>29</v>
       </c>
@@ -9300,7 +9557,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="15" t="s">
         <v>30</v>
       </c>
@@ -9344,7 +9601,7 @@
         <v>116.67</v>
       </c>
     </row>
-    <row r="53" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A53" s="15" t="s">
         <v>40</v>
       </c>
@@ -9391,7 +9648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A54" s="15" t="s">
         <v>31</v>
       </c>
@@ -9420,7 +9677,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A55" s="15" t="s">
         <v>32</v>
       </c>
@@ -9499,8 +9756,11 @@
       <c r="Z55" s="15">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="56" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA55" s="15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A56" s="15" t="s">
         <v>45</v>
       </c>
@@ -9511,7 +9771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A57" s="15" t="s">
         <v>38</v>
       </c>
@@ -9564,7 +9824,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A58" s="15" t="s">
         <v>39</v>
       </c>
@@ -9581,7 +9841,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A59" s="15" t="s">
         <v>46</v>
       </c>
@@ -9618,8 +9878,11 @@
       <c r="Y59" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA59" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A60" s="15" t="s">
         <v>49</v>
       </c>
@@ -9698,8 +9961,17 @@
       <c r="Z60" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA60" s="15">
+        <v>1</v>
+      </c>
+      <c r="AB60" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC60" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A61" s="15" t="s">
         <v>50</v>
       </c>
@@ -9778,8 +10050,17 @@
       <c r="Z61" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA61" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB61" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC61" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="15" t="s">
         <v>51</v>
       </c>
@@ -9793,7 +10074,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="63" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A63" s="15" t="s">
         <v>52</v>
       </c>
@@ -9831,7 +10112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A64" s="15" t="s">
         <v>53</v>
       </c>
@@ -9839,7 +10120,7 @@
         <v>4506429.2142857146</v>
       </c>
     </row>
-    <row r="65" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A65" s="15" t="s">
         <v>54</v>
       </c>
@@ -9918,8 +10199,17 @@
       <c r="Z65" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA65" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB65" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC65" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A66" s="9" t="s">
         <v>117</v>
       </c>
@@ -9927,7 +10217,7 @@
         <v>128340</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A67" s="9" t="s">
         <v>101</v>
       </c>
@@ -9935,13 +10225,13 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A69" s="18" t="s">
         <v>128</v>
       </c>
       <c r="E69" s="17"/>
     </row>
-    <row r="70" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A70" s="19" t="s">
         <v>129</v>
       </c>
@@ -10020,8 +10310,17 @@
       <c r="Z70" s="8" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="71" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA70" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB70" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="AC70" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A71" s="19" t="s">
         <v>130</v>
       </c>
@@ -10100,8 +10399,17 @@
       <c r="Z71" s="8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="72" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA71" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB71" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC71" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A72" s="19" t="s">
         <v>131</v>
       </c>
@@ -10180,8 +10488,17 @@
       <c r="Z72" s="8" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="73" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA72" s="28" t="s">
+        <v>1798</v>
+      </c>
+      <c r="AB72" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC72" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A73" s="19" t="s">
         <v>132</v>
       </c>
@@ -10260,8 +10577,17 @@
       <c r="Z73" s="8" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="74" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA73" s="28" t="s">
+        <v>1799</v>
+      </c>
+      <c r="AB73" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC73" s="8" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A74" s="19" t="s">
         <v>133</v>
       </c>
@@ -10340,8 +10666,17 @@
       <c r="Z74" s="8" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="75" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA74" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB74" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC74" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A75" s="19" t="s">
         <v>134</v>
       </c>
@@ -10420,8 +10755,17 @@
       <c r="Z75" s="8" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="76" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA75" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB75" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC75" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A76" s="19" t="s">
         <v>135</v>
       </c>
@@ -10500,8 +10844,17 @@
       <c r="Z76" s="8" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="77" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA76" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB76" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC76" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A77" s="19" t="s">
         <v>136</v>
       </c>
@@ -10580,8 +10933,17 @@
       <c r="Z77" s="8" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="78" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA77" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB77" s="29" t="s">
+        <v>1800</v>
+      </c>
+      <c r="AC77" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A78" s="19" t="s">
         <v>137</v>
       </c>
@@ -10660,8 +11022,17 @@
       <c r="Z78" s="8" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="79" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA78" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB78" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC78" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A79" s="19" t="s">
         <v>138</v>
       </c>
@@ -10740,8 +11111,17 @@
       <c r="Z79" s="8" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="80" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA79" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB79" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC79" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A80" s="19" t="s">
         <v>139</v>
       </c>
@@ -10820,8 +11200,17 @@
       <c r="Z80" s="8" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="81" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA80" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB80" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC80" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A81" s="19" t="s">
         <v>140</v>
       </c>
@@ -10900,8 +11289,17 @@
       <c r="Z81" s="8" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="82" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA81" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB81" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC81" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A82" s="19" t="s">
         <v>141</v>
       </c>
@@ -10980,8 +11378,17 @@
       <c r="Z82" s="8" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="83" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA82" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB82" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC82" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A83" s="19" t="s">
         <v>142</v>
       </c>
@@ -11060,8 +11467,17 @@
       <c r="Z83" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="84" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA83" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB83" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC83" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A84" s="19" t="s">
         <v>143</v>
       </c>
@@ -11137,8 +11553,17 @@
       <c r="Z84" s="8" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="85" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA84" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB84" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AC84" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A85" s="19" t="s">
         <v>144</v>
       </c>
@@ -11202,8 +11627,11 @@
       <c r="Z85" s="10" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AB85" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A86" s="19" t="s">
         <v>145</v>
       </c>
@@ -11226,26 +11654,32 @@
       <c r="T86" s="10" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AB86" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A87" s="19" t="s">
         <v>146</v>
       </c>
       <c r="F87" s="10" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AB87" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A88" s="19" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A89" s="19" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.45">
       <c r="D91" s="20"/>
       <c r="E91" s="20"/>
       <c r="F91" s="20"/>
@@ -11268,7 +11702,7 @@
       <c r="Y91" s="8"/>
       <c r="Z91" s="8"/>
     </row>
-    <row r="92" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:29" s="22" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A92" s="21" t="s">
         <v>1781</v>
       </c>
@@ -11372,8 +11806,20 @@
         <f t="shared" si="19"/>
         <v>1.0435245901639345</v>
       </c>
-    </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA92" s="22">
+        <f>SUM(AA37:AA41,AA43,AA44,AA45)</f>
+        <v>0</v>
+      </c>
+      <c r="AB92" s="22">
+        <f>SUM(AB37:AB41,AB43,AB44,AB45)</f>
+        <v>0</v>
+      </c>
+      <c r="AC92" s="22">
+        <f>SUM(AC37:AC41,AC43,AC44,AC45)</f>
+        <v>1.2202232142857146</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29" x14ac:dyDescent="0.45">
       <c r="P93" s="8"/>
       <c r="Q93" s="8"/>
       <c r="R93" s="8"/>
@@ -11383,7 +11829,7 @@
       <c r="V93" s="8"/>
       <c r="Y93" s="8"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.45">
       <c r="P94" s="8"/>
       <c r="Q94" s="8"/>
       <c r="R94" s="8"/>
@@ -11393,7 +11839,7 @@
       <c r="V94" s="8"/>
       <c r="Y94" s="8"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.45">
       <c r="P95" s="8"/>
       <c r="Q95" s="8"/>
       <c r="R95" s="8"/>
@@ -11403,7 +11849,7 @@
       <c r="V95" s="8"/>
       <c r="Y95" s="8"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.45">
       <c r="P96" s="8"/>
       <c r="Q96" s="8"/>
       <c r="R96" s="8"/>
@@ -12520,18 +12966,18 @@
       <c r="B3" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -12651,16 +13097,16 @@
       <c r="L7">
         <v>302</v>
       </c>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27"/>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27"/>
-      <c r="Y7" s="27"/>
-      <c r="Z7" s="27"/>
-      <c r="AA7" s="27"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -31462,10 +31908,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82FC352-F54F-44E2-863E-F5653510121D}">
-  <dimension ref="A1:AD282"/>
+  <dimension ref="A1:Q282"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q1048576"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31479,7 +31925,7 @@
     <col min="17" max="17" width="9.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1484</v>
       </c>
@@ -31532,7 +31978,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1712</v>
       </c>
@@ -31560,18 +32006,8 @@
       <c r="I2" s="5">
         <v>530</v>
       </c>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1713</v>
       </c>
@@ -31600,7 +32036,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1714</v>
       </c>
@@ -31629,7 +32065,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1715</v>
       </c>
@@ -31658,7 +32094,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1716</v>
       </c>
@@ -31687,7 +32123,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>1717</v>
       </c>
@@ -31716,7 +32152,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>1718</v>
       </c>
@@ -31745,7 +32181,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>1727</v>
       </c>
@@ -31774,7 +32210,7 @@
         <v>3382</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>1728</v>
       </c>
@@ -31803,7 +32239,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1719</v>
       </c>
@@ -31832,7 +32268,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>1720</v>
       </c>
@@ -31861,7 +32297,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>1721</v>
       </c>
@@ -31890,7 +32326,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>1722</v>
       </c>
@@ -31919,7 +32355,7 @@
         <v>3306</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>1723</v>
       </c>
@@ -31948,7 +32384,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>1724</v>
       </c>
@@ -39693,9 +40129,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="U2:AD2"/>
-  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -39805,16 +40238,16 @@
       <c r="I2" s="5">
         <v>530</v>
       </c>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30"/>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A3" t="s">

</xml_diff>